<commit_message>
Update Table S4 with addtional results
</commit_message>
<xml_diff>
--- a/tables/Table_S4_predictors_of_assembly_quality.xlsx
+++ b/tables/Table_S4_predictors_of_assembly_quality.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryan/Dropbox/Uni_research/Projects/Polypolish_paper/GitHub_repo/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9DB8C84-86F4-054C-9473-DDF0176E21C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A36F4FF1-367B-3045-B66F-7C57E840E8DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2300" yWindow="-26700" windowWidth="35140" windowHeight="20400" xr2:uid="{7397BC90-3645-654F-B763-2CB018FF0480}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26600" xr2:uid="{7397BC90-3645-654F-B763-2CB018FF0480}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -429,6 +429,9 @@
     <t>The average depth score provided by ALE.</t>
   </si>
   <si>
+    <t>Per-genome tau values</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -436,7 +439,7 @@
         <color theme="1"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t>Table S3:</t>
+      <t>Table S4:</t>
     </r>
     <r>
       <rPr>
@@ -446,9 +449,6 @@
       </rPr>
       <t xml:space="preserve"> For each of the 100 simulated-read genomes, we conducted a Kendall-rank correlation test using all available assemblies between the assembly's known identity (as determined by alignment to the reference) and 10 different potential predictors. Per-genome Kendall rank correlation coefficients (tau) for each predictor are shown here as a heatmap, ranging from -1 (red) to 1 (blue). The mean Kendall rank correlation coefficient (tau) for each predictor was then calculated to determine which of the predictors was overall most correlated with assembly identity. Three of the predictors were based on Prodigal gene predictions: prodigal_count, total_prodigal_length and mean_prodigal_length. Two of the predictors were based on totals from a SAM file of short-read alignments to the assembly: total_mapq and total_alignment_score. Five of the predictors came from the ALE (Assembly Likelihood Estimator) tool: ale_score, ale_place_avg, ale_insert_avg, ale_kmer_avg and ale_depth_score_avg.</t>
     </r>
-  </si>
-  <si>
-    <t>Per-genome tau values</t>
   </si>
 </sst>
 </file>
@@ -949,7 +949,7 @@
   <dimension ref="A1:CZ13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:CZ1"/>
+      <selection activeCell="AB4" sqref="AB4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -963,7 +963,7 @@
   <sheetData>
     <row r="1" spans="1:104" ht="105" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -1071,7 +1071,7 @@
     </row>
     <row r="2" spans="1:104" ht="19" x14ac:dyDescent="0.25">
       <c r="C2" s="22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
@@ -1501,7 +1501,7 @@
         <v>-0.77612289999999995</v>
       </c>
       <c r="E4" s="15">
-        <v>-0.6909497</v>
+        <v>-0.66124229999999995</v>
       </c>
       <c r="F4" s="15">
         <v>-0.5283812</v>
@@ -1510,7 +1510,7 @@
         <v>-0.61146060000000002</v>
       </c>
       <c r="H4" s="15">
-        <v>-0.72761260000000005</v>
+        <v>-0.73493920000000001</v>
       </c>
       <c r="I4" s="15">
         <v>-0.65468340000000003</v>
@@ -1531,7 +1531,7 @@
         <v>-0.74510080000000001</v>
       </c>
       <c r="O4" s="15">
-        <v>-0.70972710000000006</v>
+        <v>-0.63408059999999999</v>
       </c>
       <c r="P4" s="15">
         <v>-0.80534410000000001</v>
@@ -1540,28 +1540,28 @@
         <v>-0.69572520000000004</v>
       </c>
       <c r="R4" s="15">
-        <v>-0.69191639999999999</v>
+        <v>-0.68482719999999997</v>
       </c>
       <c r="S4" s="15">
         <v>-0.23132420000000001</v>
       </c>
       <c r="T4" s="15">
-        <v>-0.81246280000000004</v>
+        <v>-0.81963410000000003</v>
       </c>
       <c r="U4" s="15">
         <v>-0.67329070000000002</v>
       </c>
       <c r="V4" s="15">
-        <v>-0.55920639999999999</v>
+        <v>-0.52719229999999995</v>
       </c>
       <c r="W4" s="15">
-        <v>-0.77430750000000004</v>
+        <v>-0.78523120000000002</v>
       </c>
       <c r="X4" s="15">
         <v>-0.67419079999999998</v>
       </c>
       <c r="Y4" s="15">
-        <v>-0.68823420000000002</v>
+        <v>-0.65838529999999995</v>
       </c>
       <c r="Z4" s="15">
         <v>-0.77750859999999999</v>
@@ -1570,46 +1570,46 @@
         <v>-0.82302929999999996</v>
       </c>
       <c r="AB4" s="15">
-        <v>-0.6181449</v>
+        <v>-0.6139597</v>
       </c>
       <c r="AC4" s="15">
         <v>-0.75318850000000004</v>
       </c>
       <c r="AD4" s="15">
-        <v>-0.59285620000000006</v>
+        <v>-0.58319880000000002</v>
       </c>
       <c r="AE4" s="15">
-        <v>-0.81035279999999998</v>
+        <v>-0.82363839999999999</v>
       </c>
       <c r="AF4" s="15">
         <v>-0.62677570000000005</v>
       </c>
       <c r="AG4" s="15">
-        <v>-0.47505609999999998</v>
+        <v>-0.44574249999999999</v>
       </c>
       <c r="AH4" s="15">
         <v>-0.55491170000000001</v>
       </c>
       <c r="AI4" s="15">
-        <v>-0.79555319999999996</v>
+        <v>-0.81032510000000002</v>
       </c>
       <c r="AJ4" s="15">
         <v>-0.59542759999999995</v>
       </c>
       <c r="AK4" s="15">
-        <v>-0.51501929999999996</v>
+        <v>-0.48278310000000002</v>
       </c>
       <c r="AL4" s="15">
         <v>-0.54556590000000005</v>
       </c>
       <c r="AM4" s="15">
-        <v>-0.82652630000000005</v>
+        <v>-0.83372199999999996</v>
       </c>
       <c r="AN4" s="15">
-        <v>-0.7413826</v>
+        <v>-0.71391519999999997</v>
       </c>
       <c r="AO4" s="15">
-        <v>-0.73186640000000003</v>
+        <v>-0.72690690000000002</v>
       </c>
       <c r="AP4" s="15">
         <v>-0.44764989999999999</v>
@@ -1618,49 +1618,49 @@
         <v>-0.52141099999999996</v>
       </c>
       <c r="AR4" s="15">
-        <v>-0.82017410000000002</v>
+        <v>-0.81479480000000004</v>
       </c>
       <c r="AS4" s="15">
-        <v>-0.69728040000000002</v>
+        <v>-0.69701469999999999</v>
       </c>
       <c r="AT4" s="15">
-        <v>-0.7744645</v>
+        <v>-0.7425406</v>
       </c>
       <c r="AU4" s="15">
-        <v>-0.75193030000000005</v>
+        <v>-0.76081109999999996</v>
       </c>
       <c r="AV4" s="15">
-        <v>-0.72659119999999999</v>
+        <v>-0.6930328</v>
       </c>
       <c r="AW4" s="15">
         <v>-0.63471610000000001</v>
       </c>
       <c r="AX4" s="15">
-        <v>-0.88508350000000002</v>
+        <v>-0.88731510000000002</v>
       </c>
       <c r="AY4" s="15">
-        <v>-0.74309199999999997</v>
+        <v>-0.72126860000000004</v>
       </c>
       <c r="AZ4" s="15">
         <v>-0.80950699999999998</v>
       </c>
       <c r="BA4" s="15">
-        <v>-0.6999071</v>
+        <v>-0.67755679999999996</v>
       </c>
       <c r="BB4" s="15">
-        <v>-0.66876020000000003</v>
+        <v>-0.6487269</v>
       </c>
       <c r="BC4" s="15">
-        <v>-0.79866559999999998</v>
+        <v>-0.79333969999999998</v>
       </c>
       <c r="BD4" s="15">
-        <v>-0.66774449999999996</v>
+        <v>-0.65438689999999999</v>
       </c>
       <c r="BE4" s="15">
         <v>-0.70195549999999995</v>
       </c>
       <c r="BF4" s="15">
-        <v>-0.7158487</v>
+        <v>-0.70387599999999995</v>
       </c>
       <c r="BG4" s="15">
         <v>-0.661825</v>
@@ -1669,13 +1669,13 @@
         <v>-0.38668190000000002</v>
       </c>
       <c r="BI4" s="15">
-        <v>-0.80487850000000005</v>
+        <v>-0.80857049999999997</v>
       </c>
       <c r="BJ4" s="15">
-        <v>-0.76670000000000005</v>
+        <v>-0.76669889999999996</v>
       </c>
       <c r="BK4" s="15">
-        <v>-0.6627073</v>
+        <v>-0.68077759999999998</v>
       </c>
       <c r="BL4" s="15">
         <v>-0.76809039999999995</v>
@@ -1684,10 +1684,10 @@
         <v>-0.58037780000000005</v>
       </c>
       <c r="BN4" s="15">
-        <v>-0.39266259999999997</v>
+        <v>-0.42683470000000001</v>
       </c>
       <c r="BO4" s="15">
-        <v>-0.7361839</v>
+        <v>-0.69062639999999997</v>
       </c>
       <c r="BP4" s="15">
         <v>-0.76109150000000003</v>
@@ -1699,34 +1699,34 @@
         <v>-0.7681827</v>
       </c>
       <c r="BS4" s="15">
-        <v>-0.77544539999999995</v>
+        <v>-0.77811540000000001</v>
       </c>
       <c r="BT4" s="15">
-        <v>-0.72254130000000005</v>
+        <v>-0.7340911</v>
       </c>
       <c r="BU4" s="15">
-        <v>-0.63580979999999998</v>
+        <v>-0.59741960000000005</v>
       </c>
       <c r="BV4" s="15">
-        <v>-0.82637939999999999</v>
+        <v>-0.8332138</v>
       </c>
       <c r="BW4" s="15">
-        <v>-0.64794079999999998</v>
+        <v>-0.61823950000000005</v>
       </c>
       <c r="BX4" s="15">
-        <v>-0.66398429999999997</v>
+        <v>-0.66166659999999999</v>
       </c>
       <c r="BY4" s="15">
-        <v>-0.85178580000000004</v>
+        <v>-0.81617530000000005</v>
       </c>
       <c r="BZ4" s="15">
-        <v>-0.65603800000000001</v>
+        <v>-0.61439279999999996</v>
       </c>
       <c r="CA4" s="15">
-        <v>-0.7268599</v>
+        <v>-0.71369300000000002</v>
       </c>
       <c r="CB4" s="15">
-        <v>-0.48112319999999997</v>
+        <v>-0.44661849999999997</v>
       </c>
       <c r="CC4" s="15">
         <v>-0.60123459999999995</v>
@@ -1738,13 +1738,13 @@
         <v>-0.76018770000000002</v>
       </c>
       <c r="CF4" s="15">
-        <v>-0.76521249999999996</v>
+        <v>-0.77193869999999998</v>
       </c>
       <c r="CG4" s="15">
         <v>-0.62957169999999996</v>
       </c>
       <c r="CH4" s="15">
-        <v>-0.65401189999999998</v>
+        <v>-0.64779609999999999</v>
       </c>
       <c r="CI4" s="15">
         <v>-0.75364209999999998</v>
@@ -1759,19 +1759,19 @@
         <v>-0.8079906</v>
       </c>
       <c r="CM4" s="15">
-        <v>-0.76663040000000005</v>
+        <v>-0.75301059999999997</v>
       </c>
       <c r="CN4" s="15">
         <v>-0.47756939999999998</v>
       </c>
       <c r="CO4" s="15">
-        <v>-0.68980280000000005</v>
+        <v>-0.62970530000000002</v>
       </c>
       <c r="CP4" s="15">
         <v>-0.5401956</v>
       </c>
       <c r="CQ4" s="15">
-        <v>-0.80462829999999996</v>
+        <v>-0.79088579999999997</v>
       </c>
       <c r="CR4" s="15">
         <v>-0.60564249999999997</v>
@@ -1780,23 +1780,23 @@
         <v>-0.77978579999999997</v>
       </c>
       <c r="CT4" s="15">
-        <v>-0.65873159999999997</v>
+        <v>-0.62833859999999997</v>
       </c>
       <c r="CU4" s="15">
         <v>-0.73429770000000005</v>
       </c>
       <c r="CV4" s="15">
-        <v>-0.65998409999999996</v>
+        <v>-0.63254560000000004</v>
       </c>
       <c r="CW4" s="15">
-        <v>-0.75418750000000001</v>
+        <v>-0.71877539999999995</v>
       </c>
       <c r="CX4" s="15">
-        <v>-0.81494580000000005</v>
+        <v>-0.80832680000000001</v>
       </c>
       <c r="CY4" s="12">
         <f t="shared" ref="CY4:CY13" si="0">AVERAGE($C4:$CX4)</f>
-        <v>-0.68799625099999995</v>
+        <v>-0.68072577899999998</v>
       </c>
       <c r="CZ4" s="5" t="s">
         <v>127</v>
@@ -1816,7 +1816,7 @@
         <v>0.68048529999999996</v>
       </c>
       <c r="E5" s="16">
-        <v>0.3429084</v>
+        <v>0.30350759999999999</v>
       </c>
       <c r="F5" s="16">
         <v>0.49372820000000001</v>
@@ -1825,7 +1825,7 @@
         <v>0.70737329999999998</v>
       </c>
       <c r="H5" s="16">
-        <v>0.72285710000000003</v>
+        <v>0.72510019999999997</v>
       </c>
       <c r="I5" s="16">
         <v>0.46822740000000002</v>
@@ -1846,7 +1846,7 @@
         <v>0.73246319999999998</v>
       </c>
       <c r="O5" s="16">
-        <v>0.49138739999999997</v>
+        <v>0.50134049999999997</v>
       </c>
       <c r="P5" s="16">
         <v>0.79770110000000005</v>
@@ -1855,28 +1855,28 @@
         <v>0.67619050000000003</v>
       </c>
       <c r="R5" s="16">
-        <v>0.49504949999999998</v>
+        <v>0.45496540000000002</v>
       </c>
       <c r="S5" s="16">
         <v>0.26036939999999997</v>
       </c>
       <c r="T5" s="16">
-        <v>0.80511690000000002</v>
+        <v>0.80399169999999998</v>
       </c>
       <c r="U5" s="16">
         <v>0.70751869999999994</v>
       </c>
       <c r="V5" s="16">
-        <v>0.56763929999999996</v>
+        <v>0.56296299999999999</v>
       </c>
       <c r="W5" s="16">
-        <v>0.3635138</v>
+        <v>0.27790720000000002</v>
       </c>
       <c r="X5" s="16">
         <v>0.63664600000000005</v>
       </c>
       <c r="Y5" s="16">
-        <v>0.63298100000000002</v>
+        <v>0.59727799999999998</v>
       </c>
       <c r="Z5" s="16">
         <v>0.72285710000000003</v>
@@ -1885,46 +1885,46 @@
         <v>0.78796560000000004</v>
       </c>
       <c r="AB5" s="16">
-        <v>0.49293969999999998</v>
+        <v>0.49468899999999999</v>
       </c>
       <c r="AC5" s="16">
         <v>0.81092050000000004</v>
       </c>
       <c r="AD5" s="16">
-        <v>0.5775806</v>
+        <v>0.5820147</v>
       </c>
       <c r="AE5" s="16">
-        <v>0.25396829999999998</v>
+        <v>0.226601</v>
       </c>
       <c r="AF5" s="16">
         <v>0.47695850000000001</v>
       </c>
       <c r="AG5" s="16">
-        <v>0.68783070000000002</v>
+        <v>0.64039409999999997</v>
       </c>
       <c r="AH5" s="16">
         <v>0.43302180000000001</v>
       </c>
       <c r="AI5" s="16">
-        <v>0.82398780000000005</v>
+        <v>0.83486769999999999</v>
       </c>
       <c r="AJ5" s="16">
         <v>0.66897390000000001</v>
       </c>
       <c r="AK5" s="16">
-        <v>0.69363810000000004</v>
+        <v>0.68433290000000002</v>
       </c>
       <c r="AL5" s="16">
         <v>0.69468529999999995</v>
       </c>
       <c r="AM5" s="16">
-        <v>0.83001290000000005</v>
+        <v>0.83900359999999996</v>
       </c>
       <c r="AN5" s="16">
-        <v>0.74470270000000005</v>
+        <v>0.72606669999999995</v>
       </c>
       <c r="AO5" s="16">
-        <v>0.71941160000000004</v>
+        <v>0.71511389999999997</v>
       </c>
       <c r="AP5" s="16">
         <v>0.59408459999999996</v>
@@ -1933,49 +1933,49 @@
         <v>0.72194469999999999</v>
       </c>
       <c r="AR5" s="16">
-        <v>0.31567590000000001</v>
+        <v>0.25627280000000002</v>
       </c>
       <c r="AS5" s="16">
-        <v>0.44768249999999998</v>
+        <v>0.40493950000000001</v>
       </c>
       <c r="AT5" s="16">
-        <v>0.78230330000000003</v>
+        <v>0.74475709999999995</v>
       </c>
       <c r="AU5" s="16">
-        <v>0.74123260000000002</v>
+        <v>0.76495389999999996</v>
       </c>
       <c r="AV5" s="16">
-        <v>0.69029359999999995</v>
+        <v>0.68473680000000003</v>
       </c>
       <c r="AW5" s="16">
         <v>0.75838609999999995</v>
       </c>
       <c r="AX5" s="16">
-        <v>0.72744569999999997</v>
+        <v>0.72207359999999998</v>
       </c>
       <c r="AY5" s="16">
-        <v>0.67314269999999998</v>
+        <v>0.67560560000000003</v>
       </c>
       <c r="AZ5" s="16">
         <v>0.71777820000000003</v>
       </c>
       <c r="BA5" s="16">
-        <v>0.66129210000000005</v>
+        <v>0.67457049999999996</v>
       </c>
       <c r="BB5" s="16">
-        <v>0.67021509999999995</v>
+        <v>0.67982169999999997</v>
       </c>
       <c r="BC5" s="16">
-        <v>0.64387729999999999</v>
+        <v>0.62198609999999999</v>
       </c>
       <c r="BD5" s="16">
-        <v>0.30891879999999999</v>
+        <v>0.33964939999999999</v>
       </c>
       <c r="BE5" s="16">
         <v>0.70588240000000002</v>
       </c>
       <c r="BF5" s="16">
-        <v>0.76124619999999998</v>
+        <v>0.75080950000000002</v>
       </c>
       <c r="BG5" s="16">
         <v>0.4812205</v>
@@ -1984,13 +1984,13 @@
         <v>0.48140159999999999</v>
       </c>
       <c r="BI5" s="16">
-        <v>0.51474719999999996</v>
+        <v>0.48681580000000002</v>
       </c>
       <c r="BJ5" s="16">
-        <v>0.50696059999999998</v>
+        <v>0.49785869999999999</v>
       </c>
       <c r="BK5" s="16">
-        <v>0.71289130000000001</v>
+        <v>0.70702589999999998</v>
       </c>
       <c r="BL5" s="16">
         <v>0.45272600000000002</v>
@@ -1999,10 +1999,10 @@
         <v>0.71494690000000005</v>
       </c>
       <c r="BN5" s="16">
-        <v>0.40768890000000002</v>
+        <v>0.34002470000000001</v>
       </c>
       <c r="BO5" s="16">
-        <v>0.51553539999999998</v>
+        <v>0.4417064</v>
       </c>
       <c r="BP5" s="16">
         <v>0.61354640000000005</v>
@@ -2014,34 +2014,34 @@
         <v>0.7614379</v>
       </c>
       <c r="BS5" s="16">
-        <v>0.42768879999999998</v>
+        <v>0.3949202</v>
       </c>
       <c r="BT5" s="16">
-        <v>0.73410949999999997</v>
+        <v>0.73141999999999996</v>
       </c>
       <c r="BU5" s="16">
-        <v>0.51209110000000002</v>
+        <v>0.47595359999999998</v>
       </c>
       <c r="BV5" s="16">
-        <v>0.80620849999999999</v>
+        <v>0.81665989999999999</v>
       </c>
       <c r="BW5" s="16">
-        <v>0.78956340000000003</v>
+        <v>0.7949136</v>
       </c>
       <c r="BX5" s="16">
-        <v>0.54574659999999997</v>
+        <v>0.51816759999999995</v>
       </c>
       <c r="BY5" s="16">
-        <v>0.72481200000000001</v>
+        <v>0.70089860000000004</v>
       </c>
       <c r="BZ5" s="16">
-        <v>0.5224664</v>
+        <v>0.48660429999999999</v>
       </c>
       <c r="CA5" s="16">
-        <v>0.82162440000000003</v>
+        <v>0.84024909999999997</v>
       </c>
       <c r="CB5" s="16">
-        <v>0.75166599999999995</v>
+        <v>0.75402250000000004</v>
       </c>
       <c r="CC5" s="16">
         <v>0.65037929999999999</v>
@@ -2053,13 +2053,13 @@
         <v>0.60781070000000004</v>
       </c>
       <c r="CF5" s="16">
-        <v>0.81848739999999998</v>
+        <v>0.81904759999999999</v>
       </c>
       <c r="CG5" s="16">
         <v>0.61853449999999999</v>
       </c>
       <c r="CH5" s="16">
-        <v>0.68275490000000005</v>
+        <v>0.68297180000000002</v>
       </c>
       <c r="CI5" s="16">
         <v>0.71682389999999996</v>
@@ -2074,19 +2074,19 @@
         <v>0.82321560000000005</v>
       </c>
       <c r="CM5" s="16">
-        <v>0.73022759999999998</v>
+        <v>0.74148289999999994</v>
       </c>
       <c r="CN5" s="16">
         <v>0.7875373</v>
       </c>
       <c r="CO5" s="16">
-        <v>0.53692479999999998</v>
+        <v>0.51703779999999999</v>
       </c>
       <c r="CP5" s="16">
         <v>0.70917660000000005</v>
       </c>
       <c r="CQ5" s="16">
-        <v>0.58187599999999995</v>
+        <v>0.56904310000000002</v>
       </c>
       <c r="CR5" s="16">
         <v>0.4129563</v>
@@ -2095,23 +2095,23 @@
         <v>0.75336979999999998</v>
       </c>
       <c r="CT5" s="16">
-        <v>0.80818970000000001</v>
+        <v>0.81616160000000004</v>
       </c>
       <c r="CU5" s="16">
         <v>0.49916319999999997</v>
       </c>
       <c r="CV5" s="16">
-        <v>0.34158519999999998</v>
+        <v>0.30520249999999999</v>
       </c>
       <c r="CW5" s="16">
-        <v>0.81592810000000005</v>
+        <v>0.80569420000000003</v>
       </c>
       <c r="CX5" s="16">
-        <v>0.6336406</v>
+        <v>0.62715520000000002</v>
       </c>
       <c r="CY5" s="13">
         <f t="shared" si="0"/>
-        <v>0.63423548699999988</v>
+        <v>0.62672633999999983</v>
       </c>
       <c r="CZ5" s="7"/>
     </row>
@@ -2129,7 +2129,7 @@
         <v>0.78699600000000003</v>
       </c>
       <c r="E6" s="16">
-        <v>0.6218648</v>
+        <v>0.57755670000000003</v>
       </c>
       <c r="F6" s="16">
         <v>0.57741089999999995</v>
@@ -2138,7 +2138,7 @@
         <v>0.6336406</v>
       </c>
       <c r="H6" s="16">
-        <v>0.76857140000000002</v>
+        <v>0.77290899999999996</v>
       </c>
       <c r="I6" s="16">
         <v>0.63545149999999995</v>
@@ -2159,7 +2159,7 @@
         <v>0.75877919999999999</v>
       </c>
       <c r="O6" s="16">
-        <v>0.6982874</v>
+        <v>0.62934230000000002</v>
       </c>
       <c r="P6" s="16">
         <v>0.80552409999999997</v>
@@ -2168,28 +2168,28 @@
         <v>0.73333329999999997</v>
       </c>
       <c r="R6" s="16">
-        <v>0.66831680000000004</v>
+        <v>0.64434179999999996</v>
       </c>
       <c r="S6" s="16">
         <v>0.39401029999999998</v>
       </c>
       <c r="T6" s="16">
-        <v>0.84337450000000003</v>
+        <v>0.84878830000000005</v>
       </c>
       <c r="U6" s="16">
         <v>0.72286570000000006</v>
       </c>
       <c r="V6" s="16">
-        <v>0.58543100000000003</v>
+        <v>0.554871</v>
       </c>
       <c r="W6" s="16">
-        <v>0.80135210000000001</v>
+        <v>0.81511679999999997</v>
       </c>
       <c r="X6" s="16">
         <v>0.65736510000000004</v>
       </c>
       <c r="Y6" s="16">
-        <v>0.71618040000000005</v>
+        <v>0.68479659999999998</v>
       </c>
       <c r="Z6" s="16">
         <v>0.7514286</v>
@@ -2198,46 +2198,46 @@
         <v>0.83954150000000005</v>
       </c>
       <c r="AB6" s="16">
-        <v>0.68549420000000005</v>
+        <v>0.67071329999999996</v>
       </c>
       <c r="AC6" s="16">
         <v>0.78947369999999994</v>
       </c>
       <c r="AD6" s="16">
-        <v>0.58370659999999996</v>
+        <v>0.57013639999999999</v>
       </c>
       <c r="AE6" s="16">
-        <v>0.78306880000000001</v>
+        <v>0.79802960000000001</v>
       </c>
       <c r="AF6" s="16">
         <v>0.6982701</v>
       </c>
       <c r="AG6" s="16">
-        <v>0.5449735</v>
+        <v>0.50738919999999998</v>
       </c>
       <c r="AH6" s="16">
         <v>0.50000239999999996</v>
       </c>
       <c r="AI6" s="16">
-        <v>0.79955690000000001</v>
+        <v>0.81356019999999996</v>
       </c>
       <c r="AJ6" s="16">
         <v>0.61520739999999996</v>
       </c>
       <c r="AK6" s="16">
-        <v>0.51854500000000003</v>
+        <v>0.49147550000000001</v>
       </c>
       <c r="AL6" s="16">
         <v>0.60740930000000004</v>
       </c>
       <c r="AM6" s="16">
-        <v>0.84520759999999995</v>
+        <v>0.85331489999999999</v>
       </c>
       <c r="AN6" s="16">
-        <v>0.77856780000000003</v>
+        <v>0.75024049999999998</v>
       </c>
       <c r="AO6" s="16">
-        <v>0.77874449999999995</v>
+        <v>0.77509110000000003</v>
       </c>
       <c r="AP6" s="16">
         <v>0.45710889999999998</v>
@@ -2246,49 +2246,49 @@
         <v>0.56681170000000003</v>
       </c>
       <c r="AR6" s="16">
-        <v>0.81857449999999998</v>
+        <v>0.7985679</v>
       </c>
       <c r="AS6" s="16">
-        <v>0.72317940000000003</v>
+        <v>0.69629839999999998</v>
       </c>
       <c r="AT6" s="16">
-        <v>0.79372379999999998</v>
+        <v>0.76100639999999997</v>
       </c>
       <c r="AU6" s="16">
-        <v>0.76018989999999997</v>
+        <v>0.77843329999999999</v>
       </c>
       <c r="AV6" s="16">
-        <v>0.73538460000000005</v>
+        <v>0.70370370000000004</v>
       </c>
       <c r="AW6" s="16">
         <v>0.63815409999999995</v>
       </c>
       <c r="AX6" s="16">
-        <v>0.90494300000000005</v>
+        <v>0.90697669999999997</v>
       </c>
       <c r="AY6" s="16">
-        <v>0.73355289999999995</v>
+        <v>0.71492659999999997</v>
       </c>
       <c r="AZ6" s="16">
         <v>0.83572299999999999</v>
       </c>
       <c r="BA6" s="16">
-        <v>0.70276680000000002</v>
+        <v>0.6831912</v>
       </c>
       <c r="BB6" s="16">
-        <v>0.73404510000000001</v>
+        <v>0.73086629999999997</v>
       </c>
       <c r="BC6" s="16">
-        <v>0.79088020000000003</v>
+        <v>0.77102459999999995</v>
       </c>
       <c r="BD6" s="16">
-        <v>0.67197790000000002</v>
+        <v>0.66982649999999999</v>
       </c>
       <c r="BE6" s="16">
         <v>0.70588240000000002</v>
       </c>
       <c r="BF6" s="16">
-        <v>0.75201899999999999</v>
+        <v>0.75512449999999998</v>
       </c>
       <c r="BG6" s="16">
         <v>0.66124970000000005</v>
@@ -2297,13 +2297,13 @@
         <v>0.71772599999999998</v>
       </c>
       <c r="BI6" s="16">
-        <v>0.81859099999999996</v>
+        <v>0.81236450000000004</v>
       </c>
       <c r="BJ6" s="16">
-        <v>0.67388669999999995</v>
+        <v>0.65236649999999996</v>
       </c>
       <c r="BK6" s="16">
-        <v>0.67973349999999999</v>
+        <v>0.6889961</v>
       </c>
       <c r="BL6" s="16">
         <v>0.77030980000000004</v>
@@ -2312,10 +2312,10 @@
         <v>0.62249690000000002</v>
       </c>
       <c r="BN6" s="16">
-        <v>0.7153022</v>
+        <v>0.72073379999999998</v>
       </c>
       <c r="BO6" s="16">
-        <v>0.74424159999999995</v>
+        <v>0.69449839999999996</v>
       </c>
       <c r="BP6" s="16">
         <v>0.78514870000000003</v>
@@ -2327,34 +2327,34 @@
         <v>0.80160430000000005</v>
       </c>
       <c r="BS6" s="16">
-        <v>0.79357290000000003</v>
+        <v>0.7967689</v>
       </c>
       <c r="BT6" s="16">
-        <v>0.74485259999999998</v>
+        <v>0.75506859999999998</v>
       </c>
       <c r="BU6" s="16">
-        <v>0.60877959999999998</v>
+        <v>0.57046920000000001</v>
       </c>
       <c r="BV6" s="16">
-        <v>0.82926840000000002</v>
+        <v>0.83462639999999999</v>
       </c>
       <c r="BW6" s="16">
-        <v>0.6728537</v>
+        <v>0.64650010000000002</v>
       </c>
       <c r="BX6" s="16">
-        <v>0.6483527</v>
+        <v>0.6566919</v>
       </c>
       <c r="BY6" s="16">
-        <v>0.83822450000000004</v>
+        <v>0.80796420000000002</v>
       </c>
       <c r="BZ6" s="16">
-        <v>0.64354100000000003</v>
+        <v>0.60404930000000001</v>
       </c>
       <c r="CA6" s="16">
-        <v>0.82450230000000002</v>
+        <v>0.80076599999999998</v>
       </c>
       <c r="CB6" s="16">
-        <v>0.53723589999999999</v>
+        <v>0.50495199999999996</v>
       </c>
       <c r="CC6" s="16">
         <v>0.66273190000000004</v>
@@ -2366,13 +2366,13 @@
         <v>0.73684320000000003</v>
       </c>
       <c r="CF6" s="16">
-        <v>0.76806719999999995</v>
+        <v>0.77460320000000005</v>
       </c>
       <c r="CG6" s="16">
         <v>0.65301719999999996</v>
       </c>
       <c r="CH6" s="16">
-        <v>0.70304230000000001</v>
+        <v>0.69536089999999995</v>
       </c>
       <c r="CI6" s="16">
         <v>0.78106759999999997</v>
@@ -2387,19 +2387,19 @@
         <v>0.82678700000000005</v>
       </c>
       <c r="CM6" s="16">
-        <v>0.81793110000000002</v>
+        <v>0.80611580000000005</v>
       </c>
       <c r="CN6" s="16">
         <v>0.7552044</v>
       </c>
       <c r="CO6" s="16">
-        <v>0.65102139999999997</v>
+        <v>0.59753469999999997</v>
       </c>
       <c r="CP6" s="16">
         <v>0.51633030000000002</v>
       </c>
       <c r="CQ6" s="16">
-        <v>0.76311609999999996</v>
+        <v>0.75915239999999995</v>
       </c>
       <c r="CR6" s="16">
         <v>0.60163719999999998</v>
@@ -2408,23 +2408,23 @@
         <v>0.78861510000000001</v>
       </c>
       <c r="CT6" s="16">
-        <v>0.72629310000000002</v>
+        <v>0.7030303</v>
       </c>
       <c r="CU6" s="16">
         <v>0.54849809999999999</v>
       </c>
       <c r="CV6" s="16">
-        <v>0.63861579999999996</v>
+        <v>0.60115649999999998</v>
       </c>
       <c r="CW6" s="16">
-        <v>0.84598070000000003</v>
+        <v>0.81992900000000002</v>
       </c>
       <c r="CX6" s="16">
-        <v>0.86605310000000002</v>
+        <v>0.85745340000000003</v>
       </c>
       <c r="CY6" s="13">
         <f t="shared" si="0"/>
-        <v>0.70981467200000015</v>
+        <v>0.70174698800000002</v>
       </c>
       <c r="CZ6" s="7" t="s">
         <v>123</v>
@@ -2444,7 +2444,7 @@
         <v>0.42043750000000002</v>
       </c>
       <c r="E7" s="16">
-        <v>-0.41124880000000003</v>
+        <v>-0.46038509999999999</v>
       </c>
       <c r="F7" s="16">
         <v>0.64426059999999996</v>
@@ -2453,7 +2453,7 @@
         <v>-0.57918119999999995</v>
       </c>
       <c r="H7" s="16">
-        <v>-0.56573759999999995</v>
+        <v>-0.58096460000000005</v>
       </c>
       <c r="I7" s="16">
         <v>-0.42981019999999998</v>
@@ -2474,7 +2474,7 @@
         <v>4.112329E-2</v>
       </c>
       <c r="O7" s="16">
-        <v>-0.60058460000000002</v>
+        <v>-0.5401243</v>
       </c>
       <c r="P7" s="16">
         <v>-0.19630639999999999</v>
@@ -2483,28 +2483,28 @@
         <v>0.66246289999999997</v>
       </c>
       <c r="R7" s="16">
-        <v>-0.28538360000000002</v>
+        <v>-0.31704840000000001</v>
       </c>
       <c r="S7" s="16">
         <v>-0.65658689999999997</v>
       </c>
       <c r="T7" s="16">
-        <v>-0.63371710000000003</v>
+        <v>-0.64694549999999995</v>
       </c>
       <c r="U7" s="16">
         <v>-0.20857819999999999</v>
       </c>
       <c r="V7" s="16">
-        <v>-0.47467340000000002</v>
+        <v>-0.496284</v>
       </c>
       <c r="W7" s="16">
-        <v>-0.16056519999999999</v>
+        <v>-0.2142066</v>
       </c>
       <c r="X7" s="16">
         <v>-0.25039889999999998</v>
       </c>
       <c r="Y7" s="16">
-        <v>-0.29106120000000002</v>
+        <v>-0.31344159999999999</v>
       </c>
       <c r="Z7" s="16">
         <v>-2.1506620000000001E-2</v>
@@ -2513,46 +2513,46 @@
         <v>-0.31746859999999999</v>
       </c>
       <c r="AB7" s="16">
-        <v>-0.58175239999999995</v>
+        <v>-0.62688080000000002</v>
       </c>
       <c r="AC7" s="16">
         <v>-0.46247559999999999</v>
       </c>
       <c r="AD7" s="16">
-        <v>-0.53584319999999996</v>
+        <v>-0.52870329999999999</v>
       </c>
       <c r="AE7" s="16">
-        <v>-0.1885879</v>
+        <v>-0.2065015</v>
       </c>
       <c r="AF7" s="16">
         <v>3.4642119999999998E-2</v>
       </c>
       <c r="AG7" s="16">
-        <v>-0.28419879999999997</v>
+        <v>-0.31188500000000002</v>
       </c>
       <c r="AH7" s="16">
         <v>-0.141211</v>
       </c>
       <c r="AI7" s="16">
-        <v>-0.39362059999999999</v>
+        <v>-0.41325509999999999</v>
       </c>
       <c r="AJ7" s="16">
         <v>-0.68466519999999997</v>
       </c>
       <c r="AK7" s="16">
-        <v>-0.37165559999999997</v>
+        <v>-0.40565620000000002</v>
       </c>
       <c r="AL7" s="16">
         <v>-0.438915</v>
       </c>
       <c r="AM7" s="16">
-        <v>-0.48906359999999999</v>
+        <v>-0.50359149999999997</v>
       </c>
       <c r="AN7" s="16">
-        <v>-0.2103312</v>
+        <v>-0.2376316</v>
       </c>
       <c r="AO7" s="16">
-        <v>-1.8670099999999999E-2</v>
+        <v>-1.9651080000000001E-2</v>
       </c>
       <c r="AP7" s="16">
         <v>-0.46628599999999998</v>
@@ -2561,49 +2561,49 @@
         <v>-0.2456854</v>
       </c>
       <c r="AR7" s="16">
-        <v>-0.61372839999999995</v>
+        <v>-0.6192742</v>
       </c>
       <c r="AS7" s="16">
-        <v>-0.64715149999999999</v>
+        <v>-0.66999379999999997</v>
       </c>
       <c r="AT7" s="16">
-        <v>-0.5635135</v>
+        <v>-0.54172019999999999</v>
       </c>
       <c r="AU7" s="16">
-        <v>-0.33392860000000002</v>
+        <v>-0.3726119</v>
       </c>
       <c r="AV7" s="16">
-        <v>-0.46275300000000003</v>
+        <v>-0.50074479999999999</v>
       </c>
       <c r="AW7" s="16">
         <v>-0.10905140000000001</v>
       </c>
       <c r="AX7" s="16">
-        <v>-0.31059300000000001</v>
+        <v>-0.31837530000000003</v>
       </c>
       <c r="AY7" s="16">
-        <v>-0.18772469999999999</v>
+        <v>-0.20752580000000001</v>
       </c>
       <c r="AZ7" s="16">
         <v>-0.47725840000000003</v>
       </c>
       <c r="BA7" s="16">
-        <v>-0.44930989999999998</v>
+        <v>-0.46336310000000003</v>
       </c>
       <c r="BB7" s="16">
-        <v>-0.30174240000000002</v>
+        <v>-0.36237540000000001</v>
       </c>
       <c r="BC7" s="16">
-        <v>-0.28853230000000002</v>
+        <v>-0.30574499999999999</v>
       </c>
       <c r="BD7" s="16">
-        <v>-0.46179809999999999</v>
+        <v>-0.44734750000000001</v>
       </c>
       <c r="BE7" s="16">
         <v>0.25580710000000001</v>
       </c>
       <c r="BF7" s="16">
-        <v>-0.42128349999999998</v>
+        <v>-0.40488489999999999</v>
       </c>
       <c r="BG7" s="16">
         <v>-0.37443880000000002</v>
@@ -2612,13 +2612,13 @@
         <v>0.13140589999999999</v>
       </c>
       <c r="BI7" s="16">
-        <v>-0.41251070000000001</v>
+        <v>-0.43870979999999998</v>
       </c>
       <c r="BJ7" s="16">
-        <v>-0.2461071</v>
+        <v>-0.27128679999999999</v>
       </c>
       <c r="BK7" s="16">
-        <v>-0.64258999999999999</v>
+        <v>-0.66666789999999998</v>
       </c>
       <c r="BL7" s="16">
         <v>-1.70358E-2</v>
@@ -2627,10 +2627,10 @@
         <v>0.25178850000000003</v>
       </c>
       <c r="BN7" s="16">
-        <v>-0.11508699999999999</v>
+        <v>-0.13459450000000001</v>
       </c>
       <c r="BO7" s="16">
-        <v>0.1145013</v>
+        <v>5.0202410000000003E-2</v>
       </c>
       <c r="BP7" s="16">
         <v>-0.15839629999999999</v>
@@ -2642,34 +2642,34 @@
         <v>4.8129890000000002E-2</v>
       </c>
       <c r="BS7" s="16">
-        <v>-0.22506039999999999</v>
+        <v>-0.2451216</v>
       </c>
       <c r="BT7" s="16">
-        <v>-0.57302489999999995</v>
+        <v>-0.57401809999999998</v>
       </c>
       <c r="BU7" s="16">
-        <v>-0.32280399999999998</v>
+        <v>-0.34705930000000002</v>
       </c>
       <c r="BV7" s="16">
-        <v>-0.50733130000000004</v>
+        <v>-0.53169849999999996</v>
       </c>
       <c r="BW7" s="16">
-        <v>-0.44407079999999999</v>
+        <v>-0.46862599999999999</v>
       </c>
       <c r="BX7" s="16">
-        <v>-0.1988481</v>
+        <v>-0.22885639999999999</v>
       </c>
       <c r="BY7" s="16">
-        <v>-0.36021189999999997</v>
+        <v>-0.37065759999999998</v>
       </c>
       <c r="BZ7" s="16">
-        <v>-0.20610690000000001</v>
+        <v>-0.22482050000000001</v>
       </c>
       <c r="CA7" s="16">
-        <v>-0.51708670000000001</v>
+        <v>-0.55041790000000002</v>
       </c>
       <c r="CB7" s="16">
-        <v>-0.44058779999999997</v>
+        <v>-0.45771289999999998</v>
       </c>
       <c r="CC7" s="16">
         <v>0.15802079999999999</v>
@@ -2681,13 +2681,13 @@
         <v>-0.22708030000000001</v>
       </c>
       <c r="CF7" s="16">
-        <v>-0.61893419999999999</v>
+        <v>-0.62452989999999997</v>
       </c>
       <c r="CG7" s="16">
         <v>-0.42350579999999999</v>
       </c>
       <c r="CH7" s="16">
-        <v>-0.42748229999999998</v>
+        <v>-0.43464439999999999</v>
       </c>
       <c r="CI7" s="16">
         <v>-0.60976249999999999</v>
@@ -2702,19 +2702,19 @@
         <v>-0.52107999999999999</v>
       </c>
       <c r="CM7" s="16">
-        <v>-0.56580149999999996</v>
+        <v>-0.58059090000000002</v>
       </c>
       <c r="CN7" s="16">
         <v>-0.1004698</v>
       </c>
       <c r="CO7" s="16">
-        <v>-0.15779840000000001</v>
+        <v>-0.19594710000000001</v>
       </c>
       <c r="CP7" s="16">
         <v>-1.3513819999999999E-2</v>
       </c>
       <c r="CQ7" s="16">
-        <v>-0.21581439999999999</v>
+        <v>-0.2268888</v>
       </c>
       <c r="CR7" s="16">
         <v>-0.1135912</v>
@@ -2723,23 +2723,23 @@
         <v>-2.8227869999999999E-2</v>
       </c>
       <c r="CT7" s="16">
-        <v>-0.40388859999999999</v>
+        <v>-0.41700490000000001</v>
       </c>
       <c r="CU7" s="16">
         <v>-8.4895639999999994E-2</v>
       </c>
       <c r="CV7" s="16">
-        <v>-0.35616690000000001</v>
+        <v>-0.39024629999999999</v>
       </c>
       <c r="CW7" s="16">
-        <v>-0.56918690000000005</v>
+        <v>-0.56156969999999995</v>
       </c>
       <c r="CX7" s="16">
-        <v>-0.2152801</v>
+        <v>-0.2426905</v>
       </c>
       <c r="CY7" s="13">
         <f t="shared" si="0"/>
-        <v>-0.26842146649999987</v>
+        <v>-0.27847389220000002</v>
       </c>
       <c r="CZ7" s="7" t="s">
         <v>126</v>
@@ -2759,7 +2759,7 @@
         <v>0.93218990000000002</v>
       </c>
       <c r="E8" s="16">
-        <v>0.63497780000000004</v>
+        <v>0.61935499999999999</v>
       </c>
       <c r="F8" s="16">
         <v>0.86193220000000004</v>
@@ -2768,7 +2768,7 @@
         <v>0.72580650000000002</v>
       </c>
       <c r="H8" s="16">
-        <v>0.77032889999999998</v>
+        <v>0.74966949999999999</v>
       </c>
       <c r="I8" s="16">
         <v>0.72942099999999999</v>
@@ -2789,7 +2789,7 @@
         <v>0.94315899999999997</v>
       </c>
       <c r="O8" s="16">
-        <v>0.75321050000000001</v>
+        <v>0.71258339999999998</v>
       </c>
       <c r="P8" s="16">
         <v>0.74108220000000002</v>
@@ -2798,28 +2798,28 @@
         <v>0.98095239999999995</v>
       </c>
       <c r="R8" s="16">
-        <v>0.77531099999999997</v>
+        <v>0.73963330000000005</v>
       </c>
       <c r="S8" s="16">
         <v>0.78110809999999997</v>
       </c>
       <c r="T8" s="16">
-        <v>0.78887300000000005</v>
+        <v>0.76995939999999996</v>
       </c>
       <c r="U8" s="16">
         <v>0.70588280000000003</v>
       </c>
       <c r="V8" s="16">
-        <v>0.73740050000000001</v>
+        <v>0.70617280000000004</v>
       </c>
       <c r="W8" s="16">
-        <v>0.72211099999999995</v>
+        <v>0.69732439999999996</v>
       </c>
       <c r="X8" s="16">
         <v>0.86821809999999999</v>
       </c>
       <c r="Y8" s="16">
-        <v>0.89508710000000002</v>
+        <v>0.86138879999999995</v>
       </c>
       <c r="Z8" s="16">
         <v>0.83381430000000001</v>
@@ -2828,46 +2828,46 @@
         <v>0.75179419999999997</v>
       </c>
       <c r="AB8" s="16">
-        <v>0.79923040000000001</v>
+        <v>0.75429769999999996</v>
       </c>
       <c r="AC8" s="16">
         <v>0.79474259999999997</v>
       </c>
       <c r="AD8" s="16">
-        <v>0.76964410000000005</v>
+        <v>0.75488809999999995</v>
       </c>
       <c r="AE8" s="16">
-        <v>0.83736010000000005</v>
+        <v>0.80895539999999999</v>
       </c>
       <c r="AF8" s="16">
         <v>0.77832509999999999</v>
       </c>
       <c r="AG8" s="16">
-        <v>0.80423279999999997</v>
+        <v>0.76847290000000001</v>
       </c>
       <c r="AH8" s="16">
         <v>0.77520219999999995</v>
       </c>
       <c r="AI8" s="16">
-        <v>0.72465389999999996</v>
+        <v>0.69405519999999998</v>
       </c>
       <c r="AJ8" s="16">
         <v>0.71049640000000003</v>
       </c>
       <c r="AK8" s="16">
-        <v>0.74960629999999995</v>
+        <v>0.71742240000000002</v>
       </c>
       <c r="AL8" s="16">
         <v>0.76392570000000004</v>
       </c>
       <c r="AM8" s="16">
-        <v>0.80455549999999998</v>
+        <v>0.78750129999999996</v>
       </c>
       <c r="AN8" s="16">
-        <v>0.77856780000000003</v>
+        <v>0.73504570000000002</v>
       </c>
       <c r="AO8" s="16">
-        <v>0.78260929999999995</v>
+        <v>0.76798350000000004</v>
       </c>
       <c r="AP8" s="16">
         <v>0.75301289999999999</v>
@@ -2876,49 +2876,49 @@
         <v>0.68016330000000003</v>
       </c>
       <c r="AR8" s="16">
-        <v>0.73650110000000002</v>
+        <v>0.706619</v>
       </c>
       <c r="AS8" s="16">
-        <v>0.82384179999999996</v>
+        <v>0.78175150000000004</v>
       </c>
       <c r="AT8" s="16">
-        <v>0.8008535</v>
+        <v>0.78947369999999994</v>
       </c>
       <c r="AU8" s="16">
-        <v>0.75260700000000003</v>
+        <v>0.73125549999999995</v>
       </c>
       <c r="AV8" s="16">
-        <v>0.77041689999999996</v>
+        <v>0.74750430000000001</v>
       </c>
       <c r="AW8" s="16">
         <v>0.84234810000000004</v>
       </c>
       <c r="AX8" s="16">
-        <v>0.84520459999999997</v>
+        <v>0.83646149999999997</v>
       </c>
       <c r="AY8" s="16">
-        <v>0.78270320000000004</v>
+        <v>0.74485259999999998</v>
       </c>
       <c r="AZ8" s="16">
         <v>0.74789919999999999</v>
       </c>
       <c r="BA8" s="16">
-        <v>0.78250909999999996</v>
+        <v>0.75349880000000002</v>
       </c>
       <c r="BB8" s="16">
-        <v>0.83443780000000001</v>
+        <v>0.80414960000000002</v>
       </c>
       <c r="BC8" s="16">
-        <v>0.79166669999999995</v>
+        <v>0.76114079999999995</v>
       </c>
       <c r="BD8" s="16">
-        <v>0.80511180000000004</v>
+        <v>0.80732700000000002</v>
       </c>
       <c r="BE8" s="16">
         <v>0.94561499999999998</v>
       </c>
       <c r="BF8" s="16">
-        <v>0.91435429999999995</v>
+        <v>0.89827049999999997</v>
       </c>
       <c r="BG8" s="16">
         <v>0.80988740000000004</v>
@@ -2927,13 +2927,13 @@
         <v>0.85720569999999996</v>
       </c>
       <c r="BI8" s="16">
-        <v>0.76077799999999995</v>
+        <v>0.74928439999999996</v>
       </c>
       <c r="BJ8" s="16">
-        <v>0.83901329999999996</v>
+        <v>0.81662230000000002</v>
       </c>
       <c r="BK8" s="16">
-        <v>0.64857379999999998</v>
+        <v>0.61945249999999996</v>
       </c>
       <c r="BL8" s="16">
         <v>0.89193769999999994</v>
@@ -2942,10 +2942,10 @@
         <v>0.89368360000000002</v>
       </c>
       <c r="BN8" s="16">
-        <v>0.8216272</v>
+        <v>0.81783919999999999</v>
       </c>
       <c r="BO8" s="16">
-        <v>0.77790619999999999</v>
+        <v>0.74383440000000001</v>
       </c>
       <c r="BP8" s="16">
         <v>0.87383880000000003</v>
@@ -2957,34 +2957,34 @@
         <v>0.93510020000000005</v>
       </c>
       <c r="BS8" s="16">
-        <v>0.8267352</v>
+        <v>0.80462909999999999</v>
       </c>
       <c r="BT8" s="16">
-        <v>0.75716799999999995</v>
+        <v>0.74103609999999998</v>
       </c>
       <c r="BU8" s="16">
-        <v>0.73750119999999997</v>
+        <v>0.70202120000000001</v>
       </c>
       <c r="BV8" s="16">
-        <v>0.62872689999999998</v>
+        <v>0.62218839999999997</v>
       </c>
       <c r="BW8" s="16">
-        <v>0.73002549999999999</v>
+        <v>0.71008760000000004</v>
       </c>
       <c r="BX8" s="16">
-        <v>0.84120950000000005</v>
+        <v>0.82324419999999998</v>
       </c>
       <c r="BY8" s="16">
-        <v>0.75582289999999996</v>
+        <v>0.742784</v>
       </c>
       <c r="BZ8" s="16">
-        <v>0.78327559999999996</v>
+        <v>0.74240189999999995</v>
       </c>
       <c r="CA8" s="16">
-        <v>0.81486559999999997</v>
+        <v>0.79045620000000005</v>
       </c>
       <c r="CB8" s="16">
-        <v>0.78353879999999998</v>
+        <v>0.74907809999999997</v>
       </c>
       <c r="CC8" s="16">
         <v>0.87763740000000001</v>
@@ -2996,13 +2996,13 @@
         <v>0.84694119999999995</v>
       </c>
       <c r="CF8" s="16">
-        <v>0.71669879999999997</v>
+        <v>0.7006405</v>
       </c>
       <c r="CG8" s="16">
         <v>0.72060449999999998</v>
       </c>
       <c r="CH8" s="16">
-        <v>0.78097070000000002</v>
+        <v>0.7722272</v>
       </c>
       <c r="CI8" s="16">
         <v>0.74541690000000005</v>
@@ -3017,19 +3017,19 @@
         <v>0.78253119999999998</v>
       </c>
       <c r="CM8" s="16">
-        <v>0.83601930000000002</v>
+        <v>0.79928670000000002</v>
       </c>
       <c r="CN8" s="16">
         <v>0.92200800000000005</v>
       </c>
       <c r="CO8" s="16">
-        <v>0.86869180000000001</v>
+        <v>0.81677409999999995</v>
       </c>
       <c r="CP8" s="16">
         <v>0.8531417</v>
       </c>
       <c r="CQ8" s="16">
-        <v>0.7535771</v>
+        <v>0.74711170000000005</v>
       </c>
       <c r="CR8" s="16">
         <v>0.75834210000000002</v>
@@ -3038,23 +3038,23 @@
         <v>0.95427620000000002</v>
       </c>
       <c r="CT8" s="16">
-        <v>0.75646550000000001</v>
+        <v>0.71515150000000005</v>
       </c>
       <c r="CU8" s="16">
         <v>0.82943610000000001</v>
       </c>
       <c r="CV8" s="16">
-        <v>0.69963399999999998</v>
+        <v>0.66436379999999995</v>
       </c>
       <c r="CW8" s="16">
-        <v>0.69977449999999997</v>
+        <v>0.67569509999999999</v>
       </c>
       <c r="CX8" s="16">
-        <v>0.75949420000000001</v>
+        <v>0.72766459999999999</v>
       </c>
       <c r="CY8" s="13">
         <f t="shared" si="0"/>
-        <v>0.80222996599999974</v>
+        <v>0.78877823599999974</v>
       </c>
       <c r="CZ8" s="7" t="s">
         <v>129</v>
@@ -3074,7 +3074,7 @@
         <v>0.87319049999999998</v>
       </c>
       <c r="E9" s="16">
-        <v>0.7602911</v>
+        <v>0.77373800000000004</v>
       </c>
       <c r="F9" s="16">
         <v>0.99582459999999995</v>
@@ -3083,7 +3083,7 @@
         <v>0.87917199999999995</v>
       </c>
       <c r="H9" s="16">
-        <v>0.85021480000000005</v>
+        <v>0.86092789999999997</v>
       </c>
       <c r="I9" s="16">
         <v>0.82470900000000003</v>
@@ -3104,7 +3104,7 @@
         <v>0.84254169999999995</v>
       </c>
       <c r="O9" s="16">
-        <v>0.90727619999999998</v>
+        <v>0.83973580000000003</v>
       </c>
       <c r="P9" s="16">
         <v>0.83908050000000001</v>
@@ -3113,28 +3113,28 @@
         <v>1</v>
       </c>
       <c r="R9" s="16">
-        <v>0.8888916</v>
+        <v>0.89170740000000004</v>
       </c>
       <c r="S9" s="16">
         <v>0.92857389999999995</v>
       </c>
       <c r="T9" s="16">
-        <v>0.78775010000000001</v>
+        <v>0.79594670000000001</v>
       </c>
       <c r="U9" s="16">
         <v>0.888378</v>
       </c>
       <c r="V9" s="16">
-        <v>0.80264970000000002</v>
+        <v>0.81627680000000002</v>
       </c>
       <c r="W9" s="16">
-        <v>0.8785425</v>
+        <v>0.89082459999999997</v>
       </c>
       <c r="X9" s="16">
         <v>0.84699519999999995</v>
       </c>
       <c r="Y9" s="16">
-        <v>0.87682199999999999</v>
+        <v>0.87546310000000005</v>
       </c>
       <c r="Z9" s="16">
         <v>0.87303940000000002</v>
@@ -3143,46 +3143,46 @@
         <v>0.91714660000000003</v>
       </c>
       <c r="AB9" s="16">
-        <v>0.80692770000000003</v>
+        <v>0.81496500000000005</v>
       </c>
       <c r="AC9" s="16">
         <v>0.87272910000000004</v>
       </c>
       <c r="AD9" s="16">
-        <v>0.76964410000000005</v>
+        <v>0.73383540000000003</v>
       </c>
       <c r="AE9" s="16">
-        <v>0.86243389999999998</v>
+        <v>0.87192119999999995</v>
       </c>
       <c r="AF9" s="16">
         <v>0.78711209999999998</v>
       </c>
       <c r="AG9" s="16">
-        <v>0.8465608</v>
+        <v>0.85221670000000005</v>
       </c>
       <c r="AH9" s="16">
         <v>0.81425709999999996</v>
       </c>
       <c r="AI9" s="16">
-        <v>0.88642670000000001</v>
+        <v>0.89705179999999995</v>
       </c>
       <c r="AJ9" s="16">
         <v>0.7917151</v>
       </c>
       <c r="AK9" s="16">
-        <v>0.86666670000000001</v>
+        <v>0.87692309999999996</v>
       </c>
       <c r="AL9" s="16">
         <v>0.9283979</v>
       </c>
       <c r="AM9" s="16">
-        <v>0.88636360000000003</v>
+        <v>0.88591799999999998</v>
       </c>
       <c r="AN9" s="16">
-        <v>0.81048390000000003</v>
+        <v>0.81818179999999996</v>
       </c>
       <c r="AO9" s="16">
-        <v>0.86279950000000005</v>
+        <v>0.84429569999999998</v>
       </c>
       <c r="AP9" s="16">
         <v>0.90444170000000002</v>
@@ -3191,49 +3191,49 @@
         <v>0.6895886</v>
       </c>
       <c r="AR9" s="16">
-        <v>0.92026079999999999</v>
+        <v>0.90178720000000001</v>
       </c>
       <c r="AS9" s="16">
-        <v>0.78306880000000001</v>
+        <v>0.79802960000000001</v>
       </c>
       <c r="AT9" s="16">
-        <v>0.84352769999999999</v>
+        <v>0.81106610000000001</v>
       </c>
       <c r="AU9" s="16">
-        <v>0.85606059999999995</v>
+        <v>0.86700460000000001</v>
       </c>
       <c r="AV9" s="16">
-        <v>0.87076920000000002</v>
+        <v>0.88034190000000001</v>
       </c>
       <c r="AW9" s="16">
         <v>0.89298100000000002</v>
       </c>
       <c r="AX9" s="16">
-        <v>0.89563729999999997</v>
+        <v>0.88035850000000004</v>
       </c>
       <c r="AY9" s="16">
-        <v>0.91046859999999996</v>
+        <v>0.89365830000000002</v>
       </c>
       <c r="AZ9" s="16">
         <v>0.87226890000000001</v>
       </c>
       <c r="BA9" s="16">
-        <v>0.87586209999999998</v>
+        <v>0.87526879999999996</v>
       </c>
       <c r="BB9" s="16">
-        <v>0.87152390000000002</v>
+        <v>0.88249080000000002</v>
       </c>
       <c r="BC9" s="16">
-        <v>0.90151519999999996</v>
+        <v>0.8966132</v>
       </c>
       <c r="BD9" s="16">
-        <v>0.82802969999999998</v>
+        <v>0.79161320000000002</v>
       </c>
       <c r="BE9" s="16">
         <v>0.99582459999999995</v>
       </c>
       <c r="BF9" s="16">
-        <v>0.86866589999999999</v>
+        <v>0.84267440000000005</v>
       </c>
       <c r="BG9" s="16">
         <v>0.88699320000000004</v>
@@ -3242,13 +3242,13 @@
         <v>0.83044260000000003</v>
       </c>
       <c r="BI9" s="16">
-        <v>0.83474340000000002</v>
+        <v>0.8185789</v>
       </c>
       <c r="BJ9" s="16">
-        <v>0.94591429999999999</v>
+        <v>0.93276970000000003</v>
       </c>
       <c r="BK9" s="16">
-        <v>0.82882880000000003</v>
+        <v>0.84871790000000003</v>
       </c>
       <c r="BL9" s="16">
         <v>0.86009369999999996</v>
@@ -3257,10 +3257,10 @@
         <v>0.73960029999999999</v>
       </c>
       <c r="BN9" s="16">
-        <v>0.86262629999999996</v>
+        <v>0.85326299999999999</v>
       </c>
       <c r="BO9" s="16">
-        <v>0.69195399999999996</v>
+        <v>0.70075759999999998</v>
       </c>
       <c r="BP9" s="16">
         <v>0.91247009999999995</v>
@@ -3272,34 +3272,34 @@
         <v>0.77615959999999995</v>
       </c>
       <c r="BS9" s="16">
-        <v>0.87546310000000005</v>
+        <v>0.87917199999999995</v>
       </c>
       <c r="BT9" s="16">
-        <v>0.87616119999999997</v>
+        <v>0.87987519999999997</v>
       </c>
       <c r="BU9" s="16">
-        <v>0.8360071</v>
+        <v>0.84201680000000001</v>
       </c>
       <c r="BV9" s="16">
-        <v>0.86879430000000002</v>
+        <v>0.87591839999999999</v>
       </c>
       <c r="BW9" s="16">
-        <v>0.87563029999999997</v>
+        <v>0.88253970000000004</v>
       </c>
       <c r="BX9" s="16">
-        <v>0.90415710000000005</v>
+        <v>0.89246599999999998</v>
       </c>
       <c r="BY9" s="16">
-        <v>0.82193859999999996</v>
+        <v>0.82488790000000001</v>
       </c>
       <c r="BZ9" s="16">
-        <v>0.90494949999999996</v>
+        <v>0.90340469999999995</v>
       </c>
       <c r="CA9" s="16">
-        <v>0.8500008</v>
+        <v>0.85564839999999998</v>
       </c>
       <c r="CB9" s="16">
-        <v>0.88446919999999996</v>
+        <v>0.88752160000000002</v>
       </c>
       <c r="CC9" s="16">
         <v>0.80639839999999996</v>
@@ -3311,13 +3311,13 @@
         <v>0.92364800000000002</v>
       </c>
       <c r="CF9" s="16">
-        <v>0.86554620000000004</v>
+        <v>0.87301589999999996</v>
       </c>
       <c r="CG9" s="16">
         <v>0.86544719999999997</v>
       </c>
       <c r="CH9" s="16">
-        <v>0.89008359999999997</v>
+        <v>0.87858849999999999</v>
       </c>
       <c r="CI9" s="16">
         <v>0.87082340000000003</v>
@@ -3332,19 +3332,19 @@
         <v>0.91087340000000006</v>
       </c>
       <c r="CM9" s="16">
-        <v>0.87393399999999999</v>
+        <v>0.87778800000000001</v>
       </c>
       <c r="CN9" s="16">
         <v>0.83372710000000005</v>
       </c>
       <c r="CO9" s="16">
-        <v>0.81881040000000005</v>
+        <v>0.8328333</v>
       </c>
       <c r="CP9" s="16">
         <v>0.7851707</v>
       </c>
       <c r="CQ9" s="16">
-        <v>0.76409870000000002</v>
+        <v>0.742784</v>
       </c>
       <c r="CR9" s="16">
         <v>0.81735659999999999</v>
@@ -3353,23 +3353,23 @@
         <v>0.86111789999999999</v>
       </c>
       <c r="CT9" s="16">
-        <v>0.84822439999999999</v>
+        <v>0.85368359999999999</v>
       </c>
       <c r="CU9" s="16">
         <v>0.79599109999999995</v>
       </c>
       <c r="CV9" s="16">
-        <v>0.84796629999999995</v>
+        <v>0.85813660000000003</v>
       </c>
       <c r="CW9" s="16">
-        <v>0.9331332</v>
+        <v>0.93096109999999999</v>
       </c>
       <c r="CX9" s="16">
-        <v>0.888378</v>
+        <v>0.89558720000000003</v>
       </c>
       <c r="CY9" s="18">
         <f t="shared" si="0"/>
-        <v>0.86225363900000018</v>
+        <v>0.86139167999999999</v>
       </c>
       <c r="CZ9" s="7" t="s">
         <v>124</v>
@@ -3389,7 +3389,7 @@
         <v>0.97938939999999997</v>
       </c>
       <c r="E10" s="16">
-        <v>0.6684599</v>
+        <v>0.65475490000000003</v>
       </c>
       <c r="F10" s="16">
         <v>0.96235150000000003</v>
@@ -3398,7 +3398,7 @@
         <v>0.79032259999999999</v>
       </c>
       <c r="H10" s="16">
-        <v>0.76462269999999999</v>
+        <v>0.74437149999999996</v>
       </c>
       <c r="I10" s="16">
         <v>0.76460870000000003</v>
@@ -3419,7 +3419,7 @@
         <v>0.95049870000000003</v>
       </c>
       <c r="O10" s="16">
-        <v>0.76462269999999999</v>
+        <v>0.72317940000000003</v>
       </c>
       <c r="P10" s="16">
         <v>0.75028819999999996</v>
@@ -3428,28 +3428,28 @@
         <v>1</v>
       </c>
       <c r="R10" s="16">
-        <v>0.81481729999999997</v>
+        <v>0.77649979999999996</v>
       </c>
       <c r="S10" s="16">
         <v>0.794933</v>
       </c>
       <c r="T10" s="16">
-        <v>0.81455060000000001</v>
+        <v>0.79431660000000004</v>
       </c>
       <c r="U10" s="16">
         <v>0.70588280000000003</v>
       </c>
       <c r="V10" s="16">
-        <v>0.76556360000000001</v>
+        <v>0.73242969999999996</v>
       </c>
       <c r="W10" s="16">
-        <v>0.79945999999999995</v>
+        <v>0.77093080000000003</v>
       </c>
       <c r="X10" s="16">
         <v>0.88682280000000002</v>
       </c>
       <c r="Y10" s="16">
-        <v>0.90716180000000002</v>
+        <v>0.87762739999999995</v>
       </c>
       <c r="Z10" s="16">
         <v>0.83880259999999995</v>
@@ -3458,46 +3458,46 @@
         <v>0.80857469999999998</v>
       </c>
       <c r="AB10" s="16">
-        <v>0.7710072</v>
+        <v>0.71991950000000005</v>
       </c>
       <c r="AC10" s="16">
         <v>0.81496500000000005</v>
       </c>
       <c r="AD10" s="16">
-        <v>0.84107279999999995</v>
+        <v>0.82406109999999999</v>
       </c>
       <c r="AE10" s="16">
-        <v>0.83289420000000003</v>
+        <v>0.80494069999999995</v>
       </c>
       <c r="AF10" s="16">
         <v>0.77832509999999999</v>
       </c>
       <c r="AG10" s="16">
-        <v>0.83597880000000002</v>
+        <v>0.80295570000000005</v>
       </c>
       <c r="AH10" s="16">
         <v>0.83101670000000005</v>
       </c>
       <c r="AI10" s="16">
-        <v>0.76454310000000003</v>
+        <v>0.73465449999999999</v>
       </c>
       <c r="AJ10" s="16">
         <v>0.75949420000000001</v>
       </c>
       <c r="AK10" s="16">
-        <v>0.80936909999999995</v>
+        <v>0.77280579999999999</v>
       </c>
       <c r="AL10" s="16">
         <v>0.7798408</v>
       </c>
       <c r="AM10" s="16">
-        <v>0.82085339999999996</v>
+        <v>0.80285490000000004</v>
       </c>
       <c r="AN10" s="16">
-        <v>0.83114639999999995</v>
+        <v>0.78822729999999996</v>
       </c>
       <c r="AO10" s="16">
-        <v>0.80198270000000005</v>
+        <v>0.79075200000000001</v>
       </c>
       <c r="AP10" s="16">
         <v>0.78614550000000005</v>
@@ -3506,49 +3506,49 @@
         <v>0.68016330000000003</v>
       </c>
       <c r="AR10" s="16">
-        <v>0.71922249999999999</v>
+        <v>0.69946330000000001</v>
       </c>
       <c r="AS10" s="16">
-        <v>0.86772490000000002</v>
+        <v>0.83251229999999998</v>
       </c>
       <c r="AT10" s="16">
-        <v>0.85490750000000004</v>
+        <v>0.84345479999999995</v>
       </c>
       <c r="AU10" s="16">
-        <v>0.80568759999999995</v>
+        <v>0.77843329999999999</v>
       </c>
       <c r="AV10" s="16">
-        <v>0.77230770000000004</v>
+        <v>0.73789170000000004</v>
       </c>
       <c r="AW10" s="16">
         <v>0.8561571</v>
       </c>
       <c r="AX10" s="16">
-        <v>0.86527670000000001</v>
+        <v>0.85535850000000002</v>
       </c>
       <c r="AY10" s="16">
-        <v>0.80259320000000001</v>
+        <v>0.7828446</v>
       </c>
       <c r="AZ10" s="16">
         <v>0.77478990000000003</v>
       </c>
       <c r="BA10" s="16">
-        <v>0.8561571</v>
+        <v>0.83100160000000001</v>
       </c>
       <c r="BB10" s="16">
-        <v>0.91920610000000003</v>
+        <v>0.89631570000000005</v>
       </c>
       <c r="BC10" s="16">
-        <v>0.86363639999999997</v>
+        <v>0.83957219999999999</v>
       </c>
       <c r="BD10" s="16">
-        <v>0.827094</v>
+        <v>0.83954130000000005</v>
       </c>
       <c r="BE10" s="16">
         <v>0.99582459999999995</v>
       </c>
       <c r="BF10" s="16">
-        <v>0.92485609999999996</v>
+        <v>0.9167573</v>
       </c>
       <c r="BG10" s="16">
         <v>0.83270109999999997</v>
@@ -3557,13 +3557,13 @@
         <v>0.86539460000000001</v>
       </c>
       <c r="BI10" s="16">
-        <v>0.79223089999999996</v>
+        <v>0.77682720000000005</v>
       </c>
       <c r="BJ10" s="16">
-        <v>0.83463030000000005</v>
+        <v>0.81259689999999996</v>
       </c>
       <c r="BK10" s="16">
-        <v>0.7330392</v>
+        <v>0.7096015</v>
       </c>
       <c r="BL10" s="16">
         <v>0.88518059999999998</v>
@@ -3572,10 +3572,10 @@
         <v>0.90601030000000005</v>
       </c>
       <c r="BN10" s="16">
-        <v>0.85194550000000002</v>
+        <v>0.84656180000000003</v>
       </c>
       <c r="BO10" s="16">
-        <v>0.77471259999999997</v>
+        <v>0.74242419999999998</v>
       </c>
       <c r="BP10" s="16">
         <v>0.94820800000000005</v>
@@ -3587,34 +3587,34 @@
         <v>0.94569619999999999</v>
       </c>
       <c r="BS10" s="16">
-        <v>0.81975310000000001</v>
+        <v>0.79815510000000001</v>
       </c>
       <c r="BT10" s="16">
-        <v>0.81787639999999995</v>
+        <v>0.80478110000000003</v>
       </c>
       <c r="BU10" s="16">
-        <v>0.74576299999999995</v>
+        <v>0.71320459999999997</v>
       </c>
       <c r="BV10" s="16">
-        <v>0.64063910000000002</v>
+        <v>0.62663420000000003</v>
       </c>
       <c r="BW10" s="16">
-        <v>0.80740149999999999</v>
+        <v>0.78316149999999995</v>
       </c>
       <c r="BX10" s="16">
-        <v>0.85837699999999995</v>
+        <v>0.83807750000000003</v>
       </c>
       <c r="BY10" s="16">
-        <v>0.76784390000000002</v>
+        <v>0.75048119999999996</v>
       </c>
       <c r="BZ10" s="16">
-        <v>0.82510099999999997</v>
+        <v>0.7889138</v>
       </c>
       <c r="CA10" s="16">
-        <v>0.82837910000000003</v>
+        <v>0.80675419999999998</v>
       </c>
       <c r="CB10" s="16">
-        <v>0.78885090000000002</v>
+        <v>0.75402250000000004</v>
       </c>
       <c r="CC10" s="16">
         <v>0.90464169999999999</v>
@@ -3626,13 +3626,13 @@
         <v>0.85944209999999999</v>
       </c>
       <c r="CF10" s="16">
-        <v>0.73905829999999995</v>
+        <v>0.72178149999999996</v>
       </c>
       <c r="CG10" s="16">
         <v>0.7793331</v>
       </c>
       <c r="CH10" s="16">
-        <v>0.79390680000000002</v>
+        <v>0.78782779999999997</v>
       </c>
       <c r="CI10" s="16">
         <v>0.7591793</v>
@@ -3647,19 +3647,19 @@
         <v>0.7932264</v>
       </c>
       <c r="CM10" s="16">
-        <v>0.86255959999999998</v>
+        <v>0.82426440000000001</v>
       </c>
       <c r="CN10" s="16">
         <v>0.92200800000000005</v>
       </c>
       <c r="CO10" s="16">
-        <v>0.83502160000000003</v>
+        <v>0.78571809999999997</v>
       </c>
       <c r="CP10" s="16">
         <v>0.8156409</v>
       </c>
       <c r="CQ10" s="16">
-        <v>0.82670909999999997</v>
+        <v>0.82670089999999996</v>
       </c>
       <c r="CR10" s="16">
         <v>0.79595959999999999</v>
@@ -3668,23 +3668,23 @@
         <v>0.98810299999999995</v>
       </c>
       <c r="CT10" s="16">
-        <v>0.77072169999999995</v>
+        <v>0.72855740000000002</v>
       </c>
       <c r="CU10" s="16">
         <v>0.82274709999999995</v>
       </c>
       <c r="CV10" s="16">
-        <v>0.74907809999999997</v>
+        <v>0.70588660000000003</v>
       </c>
       <c r="CW10" s="16">
-        <v>0.74380190000000002</v>
+        <v>0.71743789999999996</v>
       </c>
       <c r="CX10" s="16">
-        <v>0.7917151</v>
+        <v>0.76211019999999996</v>
       </c>
       <c r="CY10" s="13">
         <f t="shared" si="0"/>
-        <v>0.82914275700000006</v>
+        <v>0.81609294200000027</v>
       </c>
       <c r="CZ10" s="7" t="s">
         <v>125</v>
@@ -3704,7 +3704,7 @@
         <v>0.1222265</v>
       </c>
       <c r="E11" s="16">
-        <v>0.22053629999999999</v>
+        <v>0.22773789999999999</v>
       </c>
       <c r="F11" s="16">
         <v>0.16033900000000001</v>
@@ -3713,7 +3713,7 @@
         <v>0.32165300000000002</v>
       </c>
       <c r="H11" s="16">
-        <v>0.71099630000000003</v>
+        <v>0.70870999999999995</v>
       </c>
       <c r="I11" s="16">
         <v>0.3545181</v>
@@ -3734,7 +3734,7 @@
         <v>0.81110709999999997</v>
       </c>
       <c r="O11" s="16">
-        <v>0.55368759999999995</v>
+        <v>0.52105009999999996</v>
       </c>
       <c r="P11" s="16">
         <v>0.39210630000000002</v>
@@ -3743,28 +3743,28 @@
         <v>0.56733389999999995</v>
       </c>
       <c r="R11" s="16">
-        <v>0.26631450000000001</v>
+        <v>0.24263080000000001</v>
       </c>
       <c r="S11" s="16">
         <v>0.32668370000000002</v>
       </c>
       <c r="T11" s="16">
-        <v>0.5246442</v>
+        <v>0.5073725</v>
       </c>
       <c r="U11" s="16">
         <v>-4.0432290000000003E-2</v>
       </c>
       <c r="V11" s="16">
-        <v>0.2318363</v>
+        <v>0.22674630000000001</v>
       </c>
       <c r="W11" s="16">
-        <v>0.55091199999999996</v>
+        <v>0.51076710000000003</v>
       </c>
       <c r="X11" s="16">
         <v>7.2622690000000004E-2</v>
       </c>
       <c r="Y11" s="16">
-        <v>0.30898530000000002</v>
+        <v>0.29292099999999999</v>
       </c>
       <c r="Z11" s="16">
         <v>-0.17948939999999999</v>
@@ -3773,46 +3773,46 @@
         <v>0.24140900000000001</v>
       </c>
       <c r="AB11" s="16">
-        <v>0.56446209999999997</v>
+        <v>0.54421169999999996</v>
       </c>
       <c r="AC11" s="16">
         <v>0.21972939999999999</v>
       </c>
       <c r="AD11" s="16">
-        <v>0.1387448</v>
+        <v>0.13572049999999999</v>
       </c>
       <c r="AE11" s="16">
-        <v>0.21326909999999999</v>
+        <v>0.1982785</v>
       </c>
       <c r="AF11" s="16">
         <v>0.12817029999999999</v>
       </c>
       <c r="AG11" s="16">
-        <v>0.69014980000000004</v>
+        <v>0.7102889</v>
       </c>
       <c r="AH11" s="16">
         <v>0.32187660000000001</v>
       </c>
       <c r="AI11" s="16">
-        <v>0.72347430000000001</v>
+        <v>0.65377879999999999</v>
       </c>
       <c r="AJ11" s="16">
         <v>0.43617529999999999</v>
       </c>
       <c r="AK11" s="16">
-        <v>5.4623100000000001E-2</v>
+        <v>4.4249770000000001E-2</v>
       </c>
       <c r="AL11" s="16">
         <v>0.54559970000000002</v>
       </c>
       <c r="AM11" s="16">
-        <v>0.2192567</v>
+        <v>0.2031126</v>
       </c>
       <c r="AN11" s="16">
-        <v>0.6815542</v>
+        <v>0.68447659999999999</v>
       </c>
       <c r="AO11" s="16">
-        <v>0.42363620000000002</v>
+        <v>0.40353559999999999</v>
       </c>
       <c r="AP11" s="16">
         <v>-0.23814859999999999</v>
@@ -3821,49 +3821,49 @@
         <v>-1.5633770000000002E-2</v>
       </c>
       <c r="AR11" s="16">
-        <v>-6.8115389999999998E-2</v>
+        <v>-9.0937050000000005E-2</v>
       </c>
       <c r="AS11" s="16">
-        <v>4.6277400000000003E-2</v>
+        <v>2.2883210000000001E-2</v>
       </c>
       <c r="AT11" s="16">
-        <v>0.75286410000000004</v>
+        <v>0.76016890000000004</v>
       </c>
       <c r="AU11" s="16">
-        <v>0.38014779999999998</v>
+        <v>0.35709600000000002</v>
       </c>
       <c r="AV11" s="16">
-        <v>6.6267160000000006E-2</v>
+        <v>6.4253370000000004E-2</v>
       </c>
       <c r="AW11" s="16">
         <v>0.44878020000000002</v>
       </c>
       <c r="AX11" s="16">
-        <v>0.36769000000000002</v>
+        <v>0.36778319999999998</v>
       </c>
       <c r="AY11" s="16">
-        <v>0</v>
+        <v>-1.0900190000000001E-2</v>
       </c>
       <c r="AZ11" s="16">
         <v>0.75974620000000004</v>
       </c>
       <c r="BA11" s="16">
-        <v>0.6380034</v>
+        <v>0.62819840000000005</v>
       </c>
       <c r="BB11" s="16">
-        <v>0.32485589999999998</v>
+        <v>0.34042149999999999</v>
       </c>
       <c r="BC11" s="16">
-        <v>0.2321609</v>
+        <v>0.22934959999999999</v>
       </c>
       <c r="BD11" s="16">
-        <v>0.54568649999999996</v>
+        <v>0.50753789999999999</v>
       </c>
       <c r="BE11" s="16">
         <v>0.38655460000000003</v>
       </c>
       <c r="BF11" s="16">
-        <v>0.1606098</v>
+        <v>0.16208819999999999</v>
       </c>
       <c r="BG11" s="16">
         <v>-7.7815449999999994E-2</v>
@@ -3872,13 +3872,13 @@
         <v>0.22332469999999999</v>
       </c>
       <c r="BI11" s="16">
-        <v>5.1322270000000003E-2</v>
+        <v>2.2708760000000001E-2</v>
       </c>
       <c r="BJ11" s="16">
-        <v>0.59010430000000003</v>
+        <v>0.58441330000000002</v>
       </c>
       <c r="BK11" s="16">
-        <v>0.1512839</v>
+        <v>0.16495760000000001</v>
       </c>
       <c r="BL11" s="16">
         <v>0.22171099999999999</v>
@@ -3887,10 +3887,10 @@
         <v>0.72375610000000001</v>
       </c>
       <c r="BN11" s="16">
-        <v>0.35143619999999998</v>
+        <v>0.24754399999999999</v>
       </c>
       <c r="BO11" s="16">
-        <v>0.10945870000000001</v>
+        <v>5.3028100000000002E-2</v>
       </c>
       <c r="BP11" s="16">
         <v>0.27111639999999998</v>
@@ -3902,34 +3902,34 @@
         <v>0.33596130000000002</v>
       </c>
       <c r="BS11" s="16">
-        <v>0.1790506</v>
+        <v>0.1688511</v>
       </c>
       <c r="BT11" s="16">
-        <v>0.42863610000000002</v>
+        <v>0.41786420000000002</v>
       </c>
       <c r="BU11" s="16">
-        <v>0.15752659999999999</v>
+        <v>0.1414656</v>
       </c>
       <c r="BV11" s="16">
-        <v>0.60343119999999995</v>
+        <v>0.59936979999999995</v>
       </c>
       <c r="BW11" s="16">
-        <v>0.42143609999999998</v>
+        <v>0.4141513</v>
       </c>
       <c r="BX11" s="16">
-        <v>7.2838550000000002E-2</v>
+        <v>6.2169370000000002E-2</v>
       </c>
       <c r="BY11" s="16">
-        <v>7.4203199999999997E-2</v>
+        <v>5.4992289999999999E-2</v>
       </c>
       <c r="BZ11" s="16">
-        <v>-7.3662500000000006E-2</v>
+        <v>-9.1167970000000001E-2</v>
       </c>
       <c r="CA11" s="16">
-        <v>0.35939209999999999</v>
+        <v>0.37851659999999998</v>
       </c>
       <c r="CB11" s="16">
-        <v>0.34282829999999997</v>
+        <v>0.3435841</v>
       </c>
       <c r="CC11" s="16">
         <v>0.72255179999999997</v>
@@ -3941,13 +3941,13 @@
         <v>0.20005999999999999</v>
       </c>
       <c r="CF11" s="16">
-        <v>0.4753423</v>
+        <v>0.4477121</v>
       </c>
       <c r="CG11" s="16">
         <v>0.23734920000000001</v>
       </c>
       <c r="CH11" s="16">
-        <v>0.3693554</v>
+        <v>0.36197889999999999</v>
       </c>
       <c r="CI11" s="16">
         <v>6.9288169999999996E-2</v>
@@ -3962,19 +3962,19 @@
         <v>0.43425960000000002</v>
       </c>
       <c r="CM11" s="16">
-        <v>0.1745063</v>
+        <v>0.16984009999999999</v>
       </c>
       <c r="CN11" s="16">
         <v>0.2787926</v>
       </c>
       <c r="CO11" s="16">
-        <v>0.1102113</v>
+        <v>7.6522129999999994E-2</v>
       </c>
       <c r="CP11" s="16">
         <v>0.15550749999999999</v>
       </c>
       <c r="CQ11" s="16">
-        <v>-0.1310201</v>
+        <v>-9.5874539999999994E-2</v>
       </c>
       <c r="CR11" s="16">
         <v>0.48968339999999999</v>
@@ -3983,23 +3983,23 @@
         <v>0.49543979999999999</v>
       </c>
       <c r="CT11" s="16">
-        <v>4.4619739999999998E-2</v>
+        <v>1.253309E-2</v>
       </c>
       <c r="CU11" s="16">
         <v>0.29629800000000001</v>
       </c>
       <c r="CV11" s="16">
-        <v>0.26417620000000003</v>
+        <v>0.27467510000000001</v>
       </c>
       <c r="CW11" s="16">
-        <v>-4.6422720000000002E-3</v>
+        <v>-1.322215E-2</v>
       </c>
       <c r="CX11" s="16">
-        <v>0.40900940000000002</v>
+        <v>0.42095870000000002</v>
       </c>
       <c r="CY11" s="13">
         <f t="shared" si="0"/>
-        <v>0.29163338138000006</v>
+        <v>0.28480067170000006</v>
       </c>
       <c r="CZ11" s="7"/>
     </row>
@@ -4017,7 +4017,7 @@
         <v>-7.8800899999999993E-2</v>
       </c>
       <c r="E12" s="16">
-        <v>-0.100753</v>
+        <v>-7.0347809999999997E-2</v>
       </c>
       <c r="F12" s="16">
         <v>7.5314469999999994E-2</v>
@@ -4026,7 +4026,7 @@
         <v>-0.19824230000000001</v>
       </c>
       <c r="H12" s="16">
-        <v>-0.22955739999999999</v>
+        <v>-0.25832430000000001</v>
       </c>
       <c r="I12" s="16">
         <v>-1.4932030000000001E-2</v>
@@ -4047,7 +4047,7 @@
         <v>-1.1090590000000001E-2</v>
       </c>
       <c r="O12" s="16">
-        <v>-0.18417739999999999</v>
+        <v>-0.1201629</v>
       </c>
       <c r="P12" s="16">
         <v>2.5165299999999999E-3</v>
@@ -4056,28 +4056,28 @@
         <v>-0.14285709999999999</v>
       </c>
       <c r="R12" s="16">
-        <v>-0.11855839999999999</v>
+        <v>-0.11837979999999999</v>
       </c>
       <c r="S12" s="16">
         <v>0.14404610000000001</v>
       </c>
       <c r="T12" s="16">
-        <v>-9.2051320000000006E-2</v>
+        <v>-7.8006880000000001E-2</v>
       </c>
       <c r="U12" s="16">
         <v>-0.23381859999999999</v>
       </c>
       <c r="V12" s="16">
-        <v>-8.3454639999999997E-2</v>
+        <v>-9.0466249999999998E-2</v>
       </c>
       <c r="W12" s="16">
-        <v>0.34179229999999999</v>
+        <v>0.36870589999999998</v>
       </c>
       <c r="X12" s="16">
         <v>-0.65540900000000002</v>
       </c>
       <c r="Y12" s="16">
-        <v>-0.3905671</v>
+        <v>-0.3737413</v>
       </c>
       <c r="Z12" s="16">
         <v>-0.86291099999999998</v>
@@ -4086,46 +4086,46 @@
         <v>7.992399E-2</v>
       </c>
       <c r="AB12" s="16">
-        <v>-0.53543830000000003</v>
+        <v>-0.43661749999999999</v>
       </c>
       <c r="AC12" s="16">
         <v>7.7042059999999996E-2</v>
       </c>
       <c r="AD12" s="16">
-        <v>-0.14299500000000001</v>
+        <v>-0.11218309999999999</v>
       </c>
       <c r="AE12" s="16">
-        <v>-0.28800920000000002</v>
+        <v>-0.2935469</v>
       </c>
       <c r="AF12" s="16">
         <v>-0.20685680000000001</v>
       </c>
       <c r="AG12" s="16">
-        <v>-0.1095964</v>
+        <v>-7.0721839999999994E-2</v>
       </c>
       <c r="AH12" s="16">
         <v>-0.12812560000000001</v>
       </c>
       <c r="AI12" s="16">
-        <v>0.12592880000000001</v>
+        <v>9.5346260000000002E-2</v>
       </c>
       <c r="AJ12" s="16">
         <v>-0.25149379999999999</v>
       </c>
       <c r="AK12" s="16">
-        <v>-5.5009130000000003E-2</v>
+        <v>-5.0902780000000002E-2</v>
       </c>
       <c r="AL12" s="16">
         <v>1.2759319999999999E-2</v>
       </c>
       <c r="AM12" s="16">
-        <v>-0.4205566</v>
+        <v>-0.42256470000000002</v>
       </c>
       <c r="AN12" s="16">
-        <v>0.43640499999999999</v>
+        <v>0.43886760000000002</v>
       </c>
       <c r="AO12" s="16">
-        <v>-0.42500650000000001</v>
+        <v>-0.4257958</v>
       </c>
       <c r="AP12" s="16">
         <v>-1.687774E-3</v>
@@ -4134,49 +4134,49 @@
         <v>-0.50622540000000005</v>
       </c>
       <c r="AR12" s="16">
-        <v>-0.18882399999999999</v>
+        <v>-0.20426320000000001</v>
       </c>
       <c r="AS12" s="16">
-        <v>-0.1739773</v>
+        <v>-0.1391135</v>
       </c>
       <c r="AT12" s="16">
-        <v>-0.54567639999999995</v>
+        <v>-0.56418199999999996</v>
       </c>
       <c r="AU12" s="16">
-        <v>-0.12896920000000001</v>
+        <v>-0.1214911</v>
       </c>
       <c r="AV12" s="16">
-        <v>-0.25833980000000001</v>
+        <v>-0.27787400000000001</v>
       </c>
       <c r="AW12" s="16">
         <v>4.6789030000000002E-2</v>
       </c>
       <c r="AX12" s="16">
-        <v>0.109136</v>
+        <v>0.1000408</v>
       </c>
       <c r="AY12" s="16">
-        <v>0.20711689999999999</v>
+        <v>0.23462069999999999</v>
       </c>
       <c r="AZ12" s="16">
         <v>6.7796640000000005E-2</v>
       </c>
       <c r="BA12" s="16">
-        <v>-0.29490709999999998</v>
+        <v>-0.30423159999999999</v>
       </c>
       <c r="BB12" s="16">
-        <v>-0.2456518</v>
+        <v>-0.28342430000000002</v>
       </c>
       <c r="BC12" s="16">
-        <v>-9.7638240000000001E-2</v>
+        <v>-0.1031282</v>
       </c>
       <c r="BD12" s="16">
-        <v>0.22785420000000001</v>
+        <v>0.1719735</v>
       </c>
       <c r="BE12" s="16">
         <v>4.2556660000000003E-2</v>
       </c>
       <c r="BF12" s="16">
-        <v>-0.22888049999999999</v>
+        <v>-0.2378991</v>
       </c>
       <c r="BG12" s="16">
         <v>-9.0871129999999994E-2</v>
@@ -4185,13 +4185,13 @@
         <v>-0.10177890000000001</v>
       </c>
       <c r="BI12" s="16">
-        <v>-0.18395729999999999</v>
+        <v>-0.19870189999999999</v>
       </c>
       <c r="BJ12" s="16">
-        <v>-0.33151239999999998</v>
+        <v>-0.32886090000000001</v>
       </c>
       <c r="BK12" s="16">
-        <v>-0.38612760000000002</v>
+        <v>-0.42370039999999998</v>
       </c>
       <c r="BL12" s="16">
         <v>-0.16833699999999999</v>
@@ -4200,10 +4200,10 @@
         <v>-0.16750509999999999</v>
       </c>
       <c r="BN12" s="16">
-        <v>8.8373419999999994E-2</v>
+        <v>0.13442950000000001</v>
       </c>
       <c r="BO12" s="16">
-        <v>0.13856560000000001</v>
+        <v>0.1570878</v>
       </c>
       <c r="BP12" s="16">
         <v>-0.54646819999999996</v>
@@ -4215,34 +4215,34 @@
         <v>-0.30298930000000002</v>
       </c>
       <c r="BS12" s="16">
-        <v>-0.3192179</v>
+        <v>-0.33063510000000002</v>
       </c>
       <c r="BT12" s="16">
-        <v>-0.21099319999999999</v>
+        <v>-0.22629869999999999</v>
       </c>
       <c r="BU12" s="16">
-        <v>-4.3823359999999999E-2</v>
+        <v>-1.968133E-2</v>
       </c>
       <c r="BV12" s="16">
-        <v>-0.3870363</v>
+        <v>-0.42149300000000001</v>
       </c>
       <c r="BW12" s="16">
-        <v>0.31522719999999999</v>
+        <v>0.32617950000000001</v>
       </c>
       <c r="BX12" s="16">
-        <v>6.9495149999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="BY12" s="16">
-        <v>-0.38054569999999999</v>
+        <v>-0.41615999999999997</v>
       </c>
       <c r="BZ12" s="16">
-        <v>-1.351132E-2</v>
+        <v>-8.4846560000000001E-3</v>
       </c>
       <c r="CA12" s="16">
-        <v>-0.49864540000000002</v>
+        <v>-0.53130710000000003</v>
       </c>
       <c r="CB12" s="16">
-        <v>-0.1160152</v>
+        <v>-0.10886419999999999</v>
       </c>
       <c r="CC12" s="16">
         <v>0.221413</v>
@@ -4254,13 +4254,13 @@
         <v>9.629894E-2</v>
       </c>
       <c r="CF12" s="16">
-        <v>-0.37680930000000001</v>
+        <v>-0.37645200000000001</v>
       </c>
       <c r="CG12" s="16">
         <v>-0.3920534</v>
       </c>
       <c r="CH12" s="16">
-        <v>0.11283319999999999</v>
+        <v>0.1042242</v>
       </c>
       <c r="CI12" s="16">
         <v>-0.198489</v>
@@ -4275,19 +4275,19 @@
         <v>-0.25072680000000003</v>
       </c>
       <c r="CM12" s="16">
-        <v>0.32206600000000002</v>
+        <v>0.33559369999999999</v>
       </c>
       <c r="CN12" s="16">
         <v>0.2045226</v>
       </c>
       <c r="CO12" s="16">
-        <v>-8.5383490000000006E-2</v>
+        <v>-5.2251899999999997E-2</v>
       </c>
       <c r="CP12" s="16">
         <v>-7.4171150000000005E-2</v>
       </c>
       <c r="CQ12" s="16">
-        <v>-3.0256069999999999E-2</v>
+        <v>-5.1684870000000001E-2</v>
       </c>
       <c r="CR12" s="16">
         <v>0.16328319999999999</v>
@@ -4296,23 +4296,23 @@
         <v>-0.1349081</v>
       </c>
       <c r="CT12" s="16">
-        <v>7.0222789999999993E-2</v>
+        <v>9.5772869999999996E-2</v>
       </c>
       <c r="CU12" s="16">
         <v>-3.801293E-2</v>
       </c>
       <c r="CV12" s="16">
-        <v>-0.1323163</v>
+        <v>-0.1153058</v>
       </c>
       <c r="CW12" s="16">
-        <v>-0.49164819999999998</v>
+        <v>-0.49812020000000001</v>
       </c>
       <c r="CX12" s="16">
-        <v>2.1232319999999999E-2</v>
+        <v>3.7454019999999998E-2</v>
       </c>
       <c r="CY12" s="13">
         <f t="shared" si="0"/>
-        <v>-0.12064114603999998</v>
+        <v>-0.11926498644999997</v>
       </c>
       <c r="CZ12" s="7" t="s">
         <v>128</v>
@@ -4332,7 +4332,7 @@
         <v>0.56639390000000001</v>
       </c>
       <c r="E13" s="17">
-        <v>0.61951880000000004</v>
+        <v>0.64143119999999998</v>
       </c>
       <c r="F13" s="17">
         <v>0.64435710000000002</v>
@@ -4341,7 +4341,7 @@
         <v>0.7165899</v>
       </c>
       <c r="H13" s="17">
-        <v>0.67332449999999999</v>
+        <v>0.68609330000000002</v>
       </c>
       <c r="I13" s="17">
         <v>0.59531769999999995</v>
@@ -4362,7 +4362,7 @@
         <v>0.68868629999999997</v>
       </c>
       <c r="O13" s="17">
-        <v>0.78970039999999997</v>
+        <v>0.73572439999999995</v>
       </c>
       <c r="P13" s="17">
         <v>0.70886119999999997</v>
@@ -4371,28 +4371,28 @@
         <v>0.6</v>
       </c>
       <c r="R13" s="17">
-        <v>0.75061960000000005</v>
+        <v>0.75345819999999997</v>
       </c>
       <c r="S13" s="17">
         <v>0.82258279999999995</v>
       </c>
       <c r="T13" s="17">
-        <v>0.65003580000000005</v>
+        <v>0.66261000000000003</v>
       </c>
       <c r="U13" s="17">
         <v>0.62903229999999999</v>
       </c>
       <c r="V13" s="17">
-        <v>0.62599470000000002</v>
+        <v>0.64691359999999998</v>
       </c>
       <c r="W13" s="17">
-        <v>0.83265860000000003</v>
+        <v>0.85133570000000003</v>
       </c>
       <c r="X13" s="17">
         <v>0.64706189999999997</v>
       </c>
       <c r="Y13" s="17">
-        <v>0.74270559999999997</v>
+        <v>0.74567899999999998</v>
       </c>
       <c r="Z13" s="17">
         <v>0.68669599999999997</v>
@@ -4401,46 +4401,46 @@
         <v>0.71919770000000005</v>
       </c>
       <c r="AB13" s="17">
-        <v>0.691469</v>
+        <v>0.71789720000000001</v>
       </c>
       <c r="AC13" s="17">
         <v>0.73279349999999999</v>
       </c>
       <c r="AD13" s="17">
-        <v>0.64343189999999995</v>
+        <v>0.6124908</v>
       </c>
       <c r="AE13" s="17">
-        <v>0.52910049999999997</v>
+        <v>0.56157639999999998</v>
       </c>
       <c r="AF13" s="17">
         <v>0.53855039999999998</v>
       </c>
       <c r="AG13" s="17">
-        <v>0.65960319999999995</v>
+        <v>0.66831119999999999</v>
       </c>
       <c r="AH13" s="17">
         <v>0.63876659999999996</v>
       </c>
       <c r="AI13" s="17">
-        <v>0.71729489999999996</v>
+        <v>0.74564799999999998</v>
       </c>
       <c r="AJ13" s="17">
         <v>0.66743430000000004</v>
       </c>
       <c r="AK13" s="17">
-        <v>0.69783070000000003</v>
+        <v>0.71494690000000005</v>
       </c>
       <c r="AL13" s="17">
         <v>0.74907349999999995</v>
       </c>
       <c r="AM13" s="17">
-        <v>0.8018961</v>
+        <v>0.80642320000000001</v>
       </c>
       <c r="AN13" s="17">
-        <v>0.65858720000000004</v>
+        <v>0.67172799999999999</v>
       </c>
       <c r="AO13" s="17">
-        <v>0.70457840000000005</v>
+        <v>0.69204569999999999</v>
       </c>
       <c r="AP13" s="17">
         <v>0.7511312</v>
@@ -4449,49 +4449,49 @@
         <v>0.52226830000000002</v>
       </c>
       <c r="AR13" s="17">
-        <v>0.76806949999999996</v>
+        <v>0.77211830000000004</v>
       </c>
       <c r="AS13" s="17">
-        <v>0.74801320000000004</v>
+        <v>0.76543439999999996</v>
       </c>
       <c r="AT13" s="17">
-        <v>0.6728307</v>
+        <v>0.6491228</v>
       </c>
       <c r="AU13" s="17">
-        <v>0.64015149999999998</v>
+        <v>0.67171809999999998</v>
       </c>
       <c r="AV13" s="17">
-        <v>0.62461540000000004</v>
+        <v>0.65242169999999999</v>
       </c>
       <c r="AW13" s="17">
         <v>0.78711209999999998</v>
       </c>
       <c r="AX13" s="17">
-        <v>0.76280970000000003</v>
+        <v>0.75535830000000004</v>
       </c>
       <c r="AY13" s="17">
-        <v>0.71490450000000005</v>
+        <v>0.71019790000000005</v>
       </c>
       <c r="AZ13" s="17">
         <v>0.82996749999999997</v>
       </c>
       <c r="BA13" s="17">
-        <v>0.68275859999999999</v>
+        <v>0.69462369999999996</v>
       </c>
       <c r="BB13" s="17">
-        <v>0.70026529999999998</v>
+        <v>0.71972369999999997</v>
       </c>
       <c r="BC13" s="17">
-        <v>0.79052169999999999</v>
+        <v>0.79215020000000003</v>
       </c>
       <c r="BD13" s="17">
-        <v>0.69960359999999999</v>
+        <v>0.65809209999999996</v>
       </c>
       <c r="BE13" s="17">
         <v>0.89540529999999996</v>
       </c>
       <c r="BF13" s="17">
-        <v>0.65202360000000004</v>
+        <v>0.63135169999999996</v>
       </c>
       <c r="BG13" s="17">
         <v>0.73764390000000002</v>
@@ -4500,13 +4500,13 @@
         <v>0.59565780000000002</v>
       </c>
       <c r="BI13" s="17">
-        <v>0.69308990000000004</v>
+        <v>0.68714920000000002</v>
       </c>
       <c r="BJ13" s="17">
-        <v>0.79753560000000001</v>
+        <v>0.79542939999999995</v>
       </c>
       <c r="BK13" s="17">
-        <v>0.74474470000000004</v>
+        <v>0.75641029999999998</v>
       </c>
       <c r="BL13" s="17">
         <v>0.65097280000000002</v>
@@ -4515,10 +4515,10 @@
         <v>0.49306680000000003</v>
       </c>
       <c r="BN13" s="17">
-        <v>0.69969700000000001</v>
+        <v>0.71250519999999995</v>
       </c>
       <c r="BO13" s="17">
-        <v>0.48443199999999997</v>
+        <v>0.4995272</v>
       </c>
       <c r="BP13" s="17">
         <v>0.7569728</v>
@@ -4530,34 +4530,34 @@
         <v>0.55511339999999998</v>
       </c>
       <c r="BS13" s="17">
-        <v>0.74074070000000003</v>
+        <v>0.75345620000000002</v>
       </c>
       <c r="BT13" s="17">
-        <v>0.71103850000000002</v>
+        <v>0.72394800000000004</v>
       </c>
       <c r="BU13" s="17">
-        <v>0.69696970000000003</v>
+        <v>0.71092440000000001</v>
       </c>
       <c r="BV13" s="17">
-        <v>0.76895789999999997</v>
+        <v>0.78399350000000001</v>
       </c>
       <c r="BW13" s="17">
-        <v>0.65601370000000003</v>
+        <v>0.67196210000000001</v>
       </c>
       <c r="BX13" s="17">
-        <v>0.7936995</v>
+        <v>0.78713109999999997</v>
       </c>
       <c r="BY13" s="17">
-        <v>0.70075189999999998</v>
+        <v>0.70860080000000003</v>
       </c>
       <c r="BZ13" s="17">
-        <v>0.74025039999999998</v>
+        <v>0.74843599999999999</v>
       </c>
       <c r="CA13" s="17">
-        <v>0.78701840000000001</v>
+        <v>0.79208040000000002</v>
       </c>
       <c r="CB13" s="17">
-        <v>0.77822659999999999</v>
+        <v>0.78368890000000002</v>
       </c>
       <c r="CC13" s="17">
         <v>0.66947719999999999</v>
@@ -4569,13 +4569,13 @@
         <v>0.6760969</v>
       </c>
       <c r="CF13" s="17">
-        <v>0.74789919999999999</v>
+        <v>0.75873020000000002</v>
       </c>
       <c r="CG13" s="17">
         <v>0.72491950000000005</v>
       </c>
       <c r="CH13" s="17">
-        <v>0.64221930000000005</v>
+        <v>0.64135229999999999</v>
       </c>
       <c r="CI13" s="17">
         <v>0.76358219999999999</v>
@@ -4590,19 +4590,19 @@
         <v>0.75757580000000002</v>
       </c>
       <c r="CM13" s="17">
-        <v>0.69070209999999999</v>
+        <v>0.70535709999999996</v>
       </c>
       <c r="CN13" s="17">
         <v>0.65509430000000002</v>
       </c>
       <c r="CO13" s="17">
-        <v>0.61075199999999996</v>
+        <v>0.64087919999999998</v>
       </c>
       <c r="CP13" s="17">
         <v>0.63467799999999996</v>
       </c>
       <c r="CQ13" s="17">
-        <v>0.54256179999999998</v>
+        <v>0.50385650000000004</v>
       </c>
       <c r="CR13" s="17">
         <v>0.73939390000000005</v>
@@ -4611,23 +4611,23 @@
         <v>0.38966279999999998</v>
       </c>
       <c r="CT13" s="17">
-        <v>0.7637545</v>
+        <v>0.77047560000000004</v>
       </c>
       <c r="CU13" s="17">
         <v>0.49246299999999998</v>
       </c>
       <c r="CV13" s="17">
-        <v>0.58064519999999997</v>
+        <v>0.60416669999999995</v>
       </c>
       <c r="CW13" s="17">
-        <v>0.82794909999999999</v>
+        <v>0.81992900000000002</v>
       </c>
       <c r="CX13" s="17">
-        <v>0.81660949999999999</v>
+        <v>0.82847939999999998</v>
       </c>
       <c r="CY13" s="14">
         <f t="shared" si="0"/>
-        <v>0.68677133700000015</v>
+        <v>0.68991051700000039</v>
       </c>
       <c r="CZ13" s="9"/>
     </row>

</xml_diff>